<commit_message>
Update case 1 and 1
add without retirement result.
</commit_message>
<xml_diff>
--- a/fc/Case1&2.xlsx
+++ b/fc/Case1&2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woongjin/Desktop/Projects/InsuranceGame/fc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\GoI\InsuranceGame\fc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E86632-CAE2-004C-B26F-CF913806FD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAE9DB5-3E2B-486F-9305-C706E59D3E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="2500" windowWidth="23880" windowHeight="16180" xr2:uid="{93EEACCD-8AF9-48DF-BEAB-81301AC67219}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93EEACCD-8AF9-48DF-BEAB-81301AC67219}"/>
   </bookViews>
   <sheets>
     <sheet name="Case_1" sheetId="1" r:id="rId1"/>
@@ -21,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>step</t>
   </si>
@@ -109,7 +100,7 @@
     <t>mt</t>
   </si>
   <si>
-    <t>END</t>
+    <t>NO REtire</t>
   </si>
 </sst>
 </file>
@@ -119,10 +110,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -225,6 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,20 +538,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AEF988-3009-472E-9717-6E6A120C3C2F}">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="77" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I50" sqref="I50"/>
+      <selection pane="topRight" activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -583,8 +584,35 @@
       <c r="K1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -605,8 +633,19 @@
       <c r="L2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>180000</v>
+      </c>
+      <c r="T2">
+        <f>M2-N2-O2-P2-Q2-R2</f>
+        <v>180000</v>
+      </c>
+      <c r="U2">
+        <f>T2</f>
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>1</v>
@@ -632,10 +671,24 @@
         <f>L2+1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>184500</v>
+      </c>
+      <c r="N3">
+        <v>5040</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T61" si="1">M3-N3-O3-P3-Q3-R3</f>
+        <v>179460</v>
+      </c>
+      <c r="U3">
+        <f>U2+T3</f>
+        <v>359460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A61" si="1">A3+1</f>
+        <f t="shared" ref="A4:A61" si="2">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -655,17 +708,34 @@
         <v>181073</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K61" si="2">K3+J4</f>
+        <f t="shared" ref="K4:K61" si="3">K3+J4</f>
         <v>540533</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L36" si="3">L3+1</f>
+        <f t="shared" ref="L4:L36" si="4">L3+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>189113</v>
+      </c>
+      <c r="N4">
+        <v>5040</v>
+      </c>
+      <c r="O4">
+        <v>3000</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>181073</v>
+      </c>
+      <c r="U4">
+        <f t="shared" ref="U4:U41" si="5">U3+T4</f>
+        <v>540533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="B5">
@@ -685,17 +755,34 @@
         <v>185800</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>726333</v>
       </c>
       <c r="L5" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>193840</v>
+      </c>
+      <c r="N5">
+        <v>5040</v>
+      </c>
+      <c r="O5">
+        <v>3000</v>
+      </c>
+      <c r="T5">
+        <f>M5-N5-O5-P5-Q5-R5</f>
+        <v>185800</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="5"/>
+        <v>726333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B6">
@@ -718,17 +805,37 @@
         <v>189720</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>916053</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>198686</v>
+      </c>
+      <c r="N6">
+        <v>5040</v>
+      </c>
+      <c r="O6">
+        <v>3000</v>
+      </c>
+      <c r="P6">
+        <v>926</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>189720</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="5"/>
+        <v>916053</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B7">
@@ -754,17 +861,40 @@
         <v>176687</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1092740</v>
       </c>
       <c r="L7" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>203653</v>
+      </c>
+      <c r="N7">
+        <v>5040</v>
+      </c>
+      <c r="O7">
+        <v>3000</v>
+      </c>
+      <c r="P7">
+        <v>926</v>
+      </c>
+      <c r="Q7">
+        <v>18000</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>176687</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="5"/>
+        <v>1092740</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B8">
@@ -790,17 +920,40 @@
         <v>181779</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1274519</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>208745</v>
+      </c>
+      <c r="N8">
+        <v>5040</v>
+      </c>
+      <c r="O8">
+        <v>3000</v>
+      </c>
+      <c r="P8">
+        <v>926</v>
+      </c>
+      <c r="Q8">
+        <v>18000</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>181779</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="5"/>
+        <v>1274519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B9">
@@ -826,17 +979,40 @@
         <v>186997</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1461516</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>213963</v>
+      </c>
+      <c r="N9">
+        <v>5040</v>
+      </c>
+      <c r="O9">
+        <v>3000</v>
+      </c>
+      <c r="P9">
+        <v>926</v>
+      </c>
+      <c r="Q9">
+        <v>18000</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>186997</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="5"/>
+        <v>1461516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B10">
@@ -862,17 +1038,40 @@
         <v>192347</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1653863</v>
       </c>
       <c r="L10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>219313</v>
+      </c>
+      <c r="N10">
+        <v>5040</v>
+      </c>
+      <c r="O10">
+        <v>3000</v>
+      </c>
+      <c r="P10">
+        <v>926</v>
+      </c>
+      <c r="Q10">
+        <v>18000</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>192347</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="5"/>
+        <v>1653863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B11">
@@ -898,17 +1097,40 @@
         <v>197829</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1851692</v>
       </c>
       <c r="L11" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>224795</v>
+      </c>
+      <c r="N11">
+        <v>5040</v>
+      </c>
+      <c r="O11">
+        <v>3000</v>
+      </c>
+      <c r="P11">
+        <v>926</v>
+      </c>
+      <c r="Q11">
+        <v>18000</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>197829</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="5"/>
+        <v>1851692</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B12">
@@ -934,17 +1156,40 @@
         <v>203449</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2055141</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>230415</v>
+      </c>
+      <c r="N12">
+        <v>5040</v>
+      </c>
+      <c r="O12">
+        <v>3000</v>
+      </c>
+      <c r="P12">
+        <v>926</v>
+      </c>
+      <c r="Q12">
+        <v>18000</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>203449</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="5"/>
+        <v>2055141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B13">
@@ -970,17 +1215,40 @@
         <v>209210</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2264351</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>236176</v>
+      </c>
+      <c r="N13">
+        <v>5040</v>
+      </c>
+      <c r="O13">
+        <v>3000</v>
+      </c>
+      <c r="P13">
+        <v>926</v>
+      </c>
+      <c r="Q13">
+        <v>18000</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>209210</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="5"/>
+        <v>2264351</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="B14">
@@ -1006,17 +1274,40 @@
         <v>215114</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2479465</v>
       </c>
       <c r="L14" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>242080</v>
+      </c>
+      <c r="N14">
+        <v>5040</v>
+      </c>
+      <c r="O14">
+        <v>3000</v>
+      </c>
+      <c r="P14">
+        <v>926</v>
+      </c>
+      <c r="Q14">
+        <v>18000</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>215114</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="5"/>
+        <v>2479465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="B15">
@@ -1042,17 +1333,40 @@
         <v>221166</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2700631</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>248132</v>
+      </c>
+      <c r="N15">
+        <v>5040</v>
+      </c>
+      <c r="O15">
+        <v>3000</v>
+      </c>
+      <c r="P15">
+        <v>926</v>
+      </c>
+      <c r="Q15">
+        <v>18000</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>221166</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="5"/>
+        <v>2700631</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B16">
@@ -1078,17 +1392,40 @@
         <v>227369</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2928000</v>
       </c>
       <c r="L16" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16">
+        <v>254335</v>
+      </c>
+      <c r="N16">
+        <v>5040</v>
+      </c>
+      <c r="O16">
+        <v>3000</v>
+      </c>
+      <c r="P16">
+        <v>926</v>
+      </c>
+      <c r="Q16">
+        <v>18000</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>227369</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="5"/>
+        <v>2928000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B17">
@@ -1114,17 +1451,40 @@
         <v>233728</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3161728</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <v>260694</v>
+      </c>
+      <c r="N17">
+        <v>5040</v>
+      </c>
+      <c r="O17">
+        <v>3000</v>
+      </c>
+      <c r="P17">
+        <v>926</v>
+      </c>
+      <c r="Q17">
+        <v>18000</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>233728</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="5"/>
+        <v>3161728</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="B18">
@@ -1150,17 +1510,40 @@
         <v>240245</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3401973</v>
       </c>
       <c r="L18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18">
+        <v>267211</v>
+      </c>
+      <c r="N18">
+        <v>5040</v>
+      </c>
+      <c r="O18">
+        <v>3000</v>
+      </c>
+      <c r="P18">
+        <v>926</v>
+      </c>
+      <c r="Q18">
+        <v>18000</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="1"/>
+        <v>240245</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="5"/>
+        <v>3401973</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="B19">
@@ -1186,17 +1569,40 @@
         <v>246925</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3648898</v>
       </c>
       <c r="L19" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>273891</v>
+      </c>
+      <c r="N19">
+        <v>5040</v>
+      </c>
+      <c r="O19">
+        <v>3000</v>
+      </c>
+      <c r="P19">
+        <v>926</v>
+      </c>
+      <c r="Q19">
+        <v>18000</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="1"/>
+        <v>246925</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="5"/>
+        <v>3648898</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B20">
@@ -1225,17 +1631,43 @@
         <v>225699</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3874597</v>
       </c>
       <c r="L20" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20">
+        <v>280739</v>
+      </c>
+      <c r="N20">
+        <v>5040</v>
+      </c>
+      <c r="O20">
+        <v>3000</v>
+      </c>
+      <c r="P20">
+        <v>926</v>
+      </c>
+      <c r="Q20">
+        <v>18000</v>
+      </c>
+      <c r="R20">
+        <v>28074</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="1"/>
+        <v>225699</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="5"/>
+        <v>3874597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B21">
@@ -1264,17 +1696,43 @@
         <v>232717</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4107314</v>
       </c>
       <c r="L21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <v>287757</v>
+      </c>
+      <c r="N21">
+        <v>5040</v>
+      </c>
+      <c r="O21">
+        <v>3000</v>
+      </c>
+      <c r="P21">
+        <v>926</v>
+      </c>
+      <c r="Q21">
+        <v>18000</v>
+      </c>
+      <c r="R21">
+        <v>28074</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="1"/>
+        <v>232717</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="5"/>
+        <v>4107314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B22">
@@ -1303,17 +1761,43 @@
         <v>239911</v>
       </c>
       <c r="K22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4347225</v>
       </c>
       <c r="L22" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>294951</v>
+      </c>
+      <c r="N22">
+        <v>5040</v>
+      </c>
+      <c r="O22">
+        <v>3000</v>
+      </c>
+      <c r="P22">
+        <v>926</v>
+      </c>
+      <c r="Q22">
+        <v>18000</v>
+      </c>
+      <c r="R22">
+        <v>28074</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="1"/>
+        <v>239911</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="5"/>
+        <v>4347225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B23">
@@ -1342,17 +1826,43 @@
         <v>247285</v>
       </c>
       <c r="K23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4594510</v>
       </c>
       <c r="L23" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <v>302325</v>
+      </c>
+      <c r="N23">
+        <v>5040</v>
+      </c>
+      <c r="O23">
+        <v>3000</v>
+      </c>
+      <c r="P23">
+        <v>926</v>
+      </c>
+      <c r="Q23">
+        <v>18000</v>
+      </c>
+      <c r="R23">
+        <v>28074</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="1"/>
+        <v>247285</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="5"/>
+        <v>4594510</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="B24">
@@ -1381,17 +1891,43 @@
         <v>254843</v>
       </c>
       <c r="K24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4849353</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24">
+        <v>309883</v>
+      </c>
+      <c r="N24">
+        <v>5040</v>
+      </c>
+      <c r="O24">
+        <v>3000</v>
+      </c>
+      <c r="P24">
+        <v>926</v>
+      </c>
+      <c r="Q24">
+        <v>18000</v>
+      </c>
+      <c r="R24">
+        <v>28074</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="1"/>
+        <v>254843</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="5"/>
+        <v>4849353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="B25">
@@ -1420,17 +1956,43 @@
         <v>262590</v>
       </c>
       <c r="K25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5111943</v>
       </c>
       <c r="L25" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <v>317630</v>
+      </c>
+      <c r="N25">
+        <v>5040</v>
+      </c>
+      <c r="O25">
+        <v>3000</v>
+      </c>
+      <c r="P25">
+        <v>926</v>
+      </c>
+      <c r="Q25">
+        <v>18000</v>
+      </c>
+      <c r="R25">
+        <v>28074</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="1"/>
+        <v>262590</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="5"/>
+        <v>5111943</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B26">
@@ -1459,17 +2021,43 @@
         <v>270531</v>
       </c>
       <c r="K26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5382474</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26">
+        <v>325571</v>
+      </c>
+      <c r="N26">
+        <v>5040</v>
+      </c>
+      <c r="O26">
+        <v>3000</v>
+      </c>
+      <c r="P26">
+        <v>926</v>
+      </c>
+      <c r="Q26">
+        <v>18000</v>
+      </c>
+      <c r="R26">
+        <v>28074</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="1"/>
+        <v>270531</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="5"/>
+        <v>5382474</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B27">
@@ -1498,17 +2086,43 @@
         <v>278670</v>
       </c>
       <c r="K27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5661144</v>
       </c>
       <c r="L27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>333710</v>
+      </c>
+      <c r="N27">
+        <v>5040</v>
+      </c>
+      <c r="O27">
+        <v>3000</v>
+      </c>
+      <c r="P27">
+        <v>926</v>
+      </c>
+      <c r="Q27">
+        <v>18000</v>
+      </c>
+      <c r="R27">
+        <v>28074</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>278670</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="5"/>
+        <v>5661144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B28">
@@ -1537,17 +2151,43 @@
         <v>287013</v>
       </c>
       <c r="K28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5948157</v>
       </c>
       <c r="L28" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <v>342053</v>
+      </c>
+      <c r="N28">
+        <v>5040</v>
+      </c>
+      <c r="O28">
+        <v>3000</v>
+      </c>
+      <c r="P28">
+        <v>926</v>
+      </c>
+      <c r="Q28">
+        <v>18000</v>
+      </c>
+      <c r="R28">
+        <v>28074</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="1"/>
+        <v>287013</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="5"/>
+        <v>5948157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B29">
@@ -1576,17 +2216,43 @@
         <v>295564</v>
       </c>
       <c r="K29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6243721</v>
       </c>
       <c r="L29" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>350604</v>
+      </c>
+      <c r="N29">
+        <v>5040</v>
+      </c>
+      <c r="O29">
+        <v>3000</v>
+      </c>
+      <c r="P29">
+        <v>926</v>
+      </c>
+      <c r="Q29">
+        <v>18000</v>
+      </c>
+      <c r="R29">
+        <v>28074</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="1"/>
+        <v>295564</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="5"/>
+        <v>6243721</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B30">
@@ -1615,17 +2281,43 @@
         <v>304329</v>
       </c>
       <c r="K30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6548050</v>
       </c>
       <c r="L30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <v>359369</v>
+      </c>
+      <c r="N30">
+        <v>5040</v>
+      </c>
+      <c r="O30">
+        <v>3000</v>
+      </c>
+      <c r="P30">
+        <v>926</v>
+      </c>
+      <c r="Q30">
+        <v>18000</v>
+      </c>
+      <c r="R30">
+        <v>28074</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="1"/>
+        <v>304329</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="5"/>
+        <v>6548050</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B31">
@@ -1654,17 +2346,43 @@
         <v>313313</v>
       </c>
       <c r="K31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6861363</v>
       </c>
       <c r="L31" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <v>368353</v>
+      </c>
+      <c r="N31">
+        <v>5040</v>
+      </c>
+      <c r="O31">
+        <v>3000</v>
+      </c>
+      <c r="P31">
+        <v>926</v>
+      </c>
+      <c r="Q31">
+        <v>18000</v>
+      </c>
+      <c r="R31">
+        <v>28074</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="1"/>
+        <v>313313</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="5"/>
+        <v>6861363</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B32">
@@ -1693,17 +2411,43 @@
         <v>830535</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7691898</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>377562</v>
+      </c>
+      <c r="N32">
+        <v>5040</v>
+      </c>
+      <c r="O32">
+        <v>3000</v>
+      </c>
+      <c r="P32">
+        <v>926</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>28074</v>
+      </c>
+      <c r="T32">
+        <f>M32-N32-O32-P32-Q32-R32+490013</f>
+        <v>830535</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="5"/>
+        <v>7691898</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B33">
@@ -1732,17 +2476,43 @@
         <v>349961</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8041859</v>
       </c>
       <c r="L33" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <v>387001</v>
+      </c>
+      <c r="N33">
+        <v>5040</v>
+      </c>
+      <c r="O33">
+        <v>3000</v>
+      </c>
+      <c r="P33">
+        <v>926</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>28074</v>
+      </c>
+      <c r="T33">
+        <f>M33-N33-O33-P33-Q33-R33</f>
+        <v>349961</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="5"/>
+        <v>8041859</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="B34">
@@ -1771,17 +2541,43 @@
         <v>359636</v>
       </c>
       <c r="K34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8401495</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>396676</v>
+      </c>
+      <c r="N34">
+        <v>5040</v>
+      </c>
+      <c r="O34">
+        <v>3000</v>
+      </c>
+      <c r="P34">
+        <v>926</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>28074</v>
+      </c>
+      <c r="T34">
+        <f t="shared" ref="T34:T92" si="6">M34-N34-O34-P34-Q34-R34</f>
+        <v>359636</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="5"/>
+        <v>8401495</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B35">
@@ -1810,17 +2606,43 @@
         <v>369553</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8771048</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <v>406593</v>
+      </c>
+      <c r="N35">
+        <v>5040</v>
+      </c>
+      <c r="O35">
+        <v>3000</v>
+      </c>
+      <c r="P35">
+        <v>926</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>28074</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="6"/>
+        <v>369553</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="5"/>
+        <v>8771048</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="B36">
@@ -1849,17 +2671,43 @@
         <v>379718</v>
       </c>
       <c r="K36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9150766</v>
       </c>
       <c r="L36" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36">
+        <v>416758</v>
+      </c>
+      <c r="N36">
+        <v>5040</v>
+      </c>
+      <c r="O36">
+        <v>3000</v>
+      </c>
+      <c r="P36">
+        <v>926</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>28074</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="6"/>
+        <v>379718</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="5"/>
+        <v>9150766</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="B37">
@@ -1888,16 +2736,42 @@
         <v>-37040</v>
       </c>
       <c r="K37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9113726</v>
       </c>
       <c r="L37" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>5040</v>
+      </c>
+      <c r="O37">
+        <v>3000</v>
+      </c>
+      <c r="P37">
+        <v>926</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>28074</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="6"/>
+        <v>-37040</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="5"/>
+        <v>9113726</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B38">
@@ -1929,16 +2803,45 @@
         <v>-337040</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8776686</v>
       </c>
       <c r="L38" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>5040</v>
+      </c>
+      <c r="O38">
+        <v>3000</v>
+      </c>
+      <c r="P38">
+        <v>926</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>28074</v>
+      </c>
+      <c r="S38">
+        <v>300000</v>
+      </c>
+      <c r="T38">
+        <f>M38-N38-O38-P38-Q38-R38-S38</f>
+        <v>-337040</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="5"/>
+        <v>8776686</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="B39">
@@ -1970,16 +2873,45 @@
         <v>-337040</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8439646</v>
       </c>
       <c r="L39" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>5040</v>
+      </c>
+      <c r="O39">
+        <v>3000</v>
+      </c>
+      <c r="P39">
+        <v>926</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>28074</v>
+      </c>
+      <c r="S39">
+        <v>300000</v>
+      </c>
+      <c r="T39">
+        <f>M39-N39-O39-P39-Q39-R39-S39</f>
+        <v>-337040</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="5"/>
+        <v>8439646</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B40">
@@ -2008,16 +2940,42 @@
         <v>-37040</v>
       </c>
       <c r="K40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8402606</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>5040</v>
+      </c>
+      <c r="O40">
+        <v>3000</v>
+      </c>
+      <c r="P40">
+        <v>926</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>28074</v>
+      </c>
+      <c r="T40">
+        <f t="shared" ref="T40:T98" si="7">M40-N40-O40-P40-Q40-R40</f>
+        <v>-37040</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="5"/>
+        <v>8402606</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B41">
@@ -2039,7 +2997,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" ref="H41:H42" si="4">28074+ROUNDUP(471523*10%, 0)</f>
+        <f t="shared" ref="H41:H42" si="8">28074+ROUNDUP(471523*10%, 0)</f>
         <v>75227</v>
       </c>
       <c r="J41">
@@ -2047,16 +3005,43 @@
         <v>-84193</v>
       </c>
       <c r="K41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8318413</v>
       </c>
       <c r="L41" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>5040</v>
+      </c>
+      <c r="O41">
+        <v>3000</v>
+      </c>
+      <c r="P41">
+        <v>926</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1">
+        <f t="shared" ref="R41:R42" si="9">28074+ROUNDUP(471523*10%, 0)</f>
+        <v>75227</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="7"/>
+        <v>-84193</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="5"/>
+        <v>8318413</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B42">
@@ -2078,7 +3063,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>75227</v>
       </c>
       <c r="I42">
@@ -2096,10 +3081,41 @@
       <c r="L42" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>5040</v>
+      </c>
+      <c r="O42">
+        <v>3000</v>
+      </c>
+      <c r="P42">
+        <v>926</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1">
+        <f t="shared" si="9"/>
+        <v>75227</v>
+      </c>
+      <c r="S42">
+        <f>U41*0.2</f>
+        <v>1663682.6</v>
+      </c>
+      <c r="T42" s="1">
+        <f>M42-N42-O42-P42-Q42-R42-S42</f>
+        <v>-1747875.6</v>
+      </c>
+      <c r="U42" s="1">
+        <f>ROUNDDOWN(U41+T42,0)</f>
+        <v>6570537</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="B43">
@@ -2132,16 +3148,46 @@
         <v>-1588799</v>
       </c>
       <c r="K43" s="1">
-        <f t="shared" ref="K43:K57" si="5">ROUNDDOWN(K42+J43, 0)</f>
+        <f t="shared" ref="K43:K57" si="10">ROUNDDOWN(K42+J43, 0)</f>
         <v>4981738</v>
       </c>
       <c r="L43" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43">
+        <v>495394</v>
+      </c>
+      <c r="N43">
+        <v>5040</v>
+      </c>
+      <c r="O43">
+        <v>3000</v>
+      </c>
+      <c r="P43">
+        <v>926</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43" s="1">
+        <f>28074+ROUNDUP(471523*10%, 0)</f>
+        <v>75227</v>
+      </c>
+      <c r="S43">
+        <v>2000000</v>
+      </c>
+      <c r="T43" s="1">
+        <f>M43-N43-O43-P43-Q43-R43-S43</f>
+        <v>-1588799</v>
+      </c>
+      <c r="U43" s="1">
+        <f t="shared" ref="U43" si="11">ROUNDDOWN(U42+T43, 0)</f>
+        <v>4981738</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="B44">
@@ -2163,7 +3209,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" ref="H44:H61" si="6">H43</f>
+        <f t="shared" ref="H44:H61" si="12">H43</f>
         <v>75227</v>
       </c>
       <c r="I44">
@@ -2181,10 +3227,41 @@
       <c r="L44" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44">
+        <v>507779</v>
+      </c>
+      <c r="N44">
+        <v>5040</v>
+      </c>
+      <c r="O44">
+        <v>3000</v>
+      </c>
+      <c r="P44">
+        <v>926</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44" s="1">
+        <f t="shared" ref="R44:R61" si="13">R43</f>
+        <v>75227</v>
+      </c>
+      <c r="S44">
+        <f>U43/2</f>
+        <v>2490869</v>
+      </c>
+      <c r="T44" s="1">
+        <f>M44-N44-O44-P44-Q44-R44-S44</f>
+        <v>-2067283</v>
+      </c>
+      <c r="U44" s="1">
+        <f>ROUNDDOWN(U43+T44, 0)</f>
+        <v>2914455</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="B45">
@@ -2206,27 +3283,57 @@
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="I45">
         <v>1000000</v>
       </c>
       <c r="J45" s="1">
-        <f t="shared" ref="J45:J59" si="7">C45-D45-E45-F45-G45-H45-I45</f>
+        <f t="shared" ref="J45:J59" si="14">C45-D45-E45-F45-G45-H45-I45</f>
         <v>-563719</v>
       </c>
       <c r="K45" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2350736</v>
       </c>
       <c r="L45" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45">
+        <v>520474</v>
+      </c>
+      <c r="N45">
+        <v>5040</v>
+      </c>
+      <c r="O45">
+        <v>3000</v>
+      </c>
+      <c r="P45">
+        <v>926</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="S45">
+        <v>1000000</v>
+      </c>
+      <c r="T45" s="1">
+        <f t="shared" ref="T45:T59" si="15">M45-N45-O45-P45-Q45-R45-S45</f>
+        <v>-563719</v>
+      </c>
+      <c r="U45" s="1">
+        <f t="shared" ref="U45:U52" si="16">ROUNDDOWN(U44+T45, 0)</f>
+        <v>2350736</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="B46" s="12">
@@ -2248,25 +3355,53 @@
         <v>0</v>
       </c>
       <c r="H46" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="I46" s="12"/>
       <c r="J46" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>449292</v>
       </c>
       <c r="K46" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2800028</v>
       </c>
       <c r="L46" s="14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46">
+        <v>533485</v>
+      </c>
+      <c r="N46" s="12">
+        <v>5040</v>
+      </c>
+      <c r="O46" s="12">
+        <v>3000</v>
+      </c>
+      <c r="P46" s="12">
+        <v>926</v>
+      </c>
+      <c r="Q46" s="12">
+        <v>0</v>
+      </c>
+      <c r="R46" s="13">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="S46" s="12"/>
+      <c r="T46" s="13">
+        <f t="shared" si="15"/>
+        <v>449292</v>
+      </c>
+      <c r="U46" s="13">
+        <f t="shared" si="16"/>
+        <v>2800028</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="B47">
@@ -2288,24 +3423,51 @@
         <v>0</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>462630</v>
       </c>
       <c r="K47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3262658</v>
       </c>
       <c r="L47" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47">
+        <v>546823</v>
+      </c>
+      <c r="N47">
+        <v>5040</v>
+      </c>
+      <c r="O47">
+        <v>3000</v>
+      </c>
+      <c r="P47">
+        <v>926</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T47" s="1">
+        <f t="shared" si="15"/>
+        <v>462630</v>
+      </c>
+      <c r="U47" s="1">
+        <f t="shared" si="16"/>
+        <v>3262658</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="B48">
@@ -2327,24 +3489,51 @@
         <v>0</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J48" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>476300</v>
       </c>
       <c r="K48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3738958</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M48">
+        <v>560493</v>
+      </c>
+      <c r="N48">
+        <v>5040</v>
+      </c>
+      <c r="O48">
+        <v>3000</v>
+      </c>
+      <c r="P48">
+        <v>926</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T48" s="1">
+        <f t="shared" si="15"/>
+        <v>476300</v>
+      </c>
+      <c r="U48" s="1">
+        <f t="shared" si="16"/>
+        <v>3738958</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="B49">
@@ -2366,27 +3555,57 @@
         <v>0</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="I49">
         <v>1000000</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-509688</v>
       </c>
       <c r="K49" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3229270</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M49">
+        <v>574505</v>
+      </c>
+      <c r="N49">
+        <v>5040</v>
+      </c>
+      <c r="O49">
+        <v>3000</v>
+      </c>
+      <c r="P49">
+        <v>926</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="S49">
+        <v>1000000</v>
+      </c>
+      <c r="T49" s="1">
+        <f t="shared" si="15"/>
+        <v>-509688</v>
+      </c>
+      <c r="U49" s="1">
+        <f t="shared" si="16"/>
+        <v>3229270</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="B50">
@@ -2408,27 +3627,57 @@
         <v>0</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="I50">
         <v>1800000</v>
       </c>
       <c r="J50" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-1295325</v>
       </c>
       <c r="K50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1933945</v>
       </c>
       <c r="L50" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M50">
+        <v>588868</v>
+      </c>
+      <c r="N50">
+        <v>5040</v>
+      </c>
+      <c r="O50">
+        <v>3000</v>
+      </c>
+      <c r="P50">
+        <v>926</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="S50">
+        <v>1800000</v>
+      </c>
+      <c r="T50" s="1">
+        <f t="shared" si="15"/>
+        <v>-1295325</v>
+      </c>
+      <c r="U50" s="1">
+        <f t="shared" si="16"/>
+        <v>1933945</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="B51">
@@ -2450,24 +3699,51 @@
         <v>0</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>519397</v>
       </c>
       <c r="K51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2453342</v>
       </c>
       <c r="L51" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M51" s="15">
+        <v>603590</v>
+      </c>
+      <c r="N51">
+        <v>5040</v>
+      </c>
+      <c r="O51">
+        <v>3000</v>
+      </c>
+      <c r="P51">
+        <v>926</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T51" s="1">
+        <f t="shared" si="15"/>
+        <v>519397</v>
+      </c>
+      <c r="U51" s="1">
+        <f t="shared" si="16"/>
+        <v>2453342</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="B52">
@@ -2489,24 +3765,51 @@
         <v>0</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-84193</v>
       </c>
       <c r="K52" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2369149</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M52" s="15">
+        <v>618680</v>
+      </c>
+      <c r="N52">
+        <v>5040</v>
+      </c>
+      <c r="O52">
+        <v>3000</v>
+      </c>
+      <c r="P52">
+        <v>926</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T52" s="1">
+        <f t="shared" si="15"/>
+        <v>534487</v>
+      </c>
+      <c r="U52" s="1">
+        <f t="shared" si="16"/>
+        <v>2987829</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="B53">
@@ -2528,14 +3831,14 @@
         <v>0</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="I53">
         <v>1800000</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-1884193</v>
       </c>
       <c r="K53" s="1">
@@ -2545,10 +3848,40 @@
       <c r="L53" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M53" s="15">
+        <v>634147</v>
+      </c>
+      <c r="N53">
+        <v>5040</v>
+      </c>
+      <c r="O53">
+        <v>3000</v>
+      </c>
+      <c r="P53">
+        <v>926</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="S53">
+        <v>1800000</v>
+      </c>
+      <c r="T53" s="1">
+        <f t="shared" si="15"/>
+        <v>-1250046</v>
+      </c>
+      <c r="U53" s="1">
+        <f>ROUNDDOWN(U52+T53, 0)</f>
+        <v>1737783</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="B54">
@@ -2570,7 +3903,7 @@
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="I54">
@@ -2578,20 +3911,51 @@
         <v>96991.200000000012</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-181184.2</v>
       </c>
       <c r="K54" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>303771</v>
       </c>
       <c r="L54" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M54" s="15">
+        <v>650000</v>
+      </c>
+      <c r="N54">
+        <v>5040</v>
+      </c>
+      <c r="O54">
+        <v>3000</v>
+      </c>
+      <c r="P54">
+        <v>926</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="S54">
+        <f>U53*0.2</f>
+        <v>347556.60000000003</v>
+      </c>
+      <c r="T54" s="1">
+        <f t="shared" si="15"/>
+        <v>218250.39999999997</v>
+      </c>
+      <c r="U54" s="1">
+        <f t="shared" ref="U54:U57" si="17">ROUNDDOWN(U53+T54, 0)</f>
+        <v>1956033</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="B55">
@@ -2613,7 +3977,7 @@
         <v>0</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="I55">
@@ -2621,20 +3985,51 @@
         <v>32500</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-116693</v>
       </c>
       <c r="K55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>187078</v>
       </c>
       <c r="L55" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M55" s="15">
+        <v>666250</v>
+      </c>
+      <c r="N55">
+        <v>5040</v>
+      </c>
+      <c r="O55">
+        <v>3000</v>
+      </c>
+      <c r="P55">
+        <v>926</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="S55">
+        <f>650000*0.05</f>
+        <v>32500</v>
+      </c>
+      <c r="T55" s="1">
+        <f t="shared" si="15"/>
+        <v>549557</v>
+      </c>
+      <c r="U55" s="1">
+        <f t="shared" si="17"/>
+        <v>2505590</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="B56">
@@ -2656,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="I56">
@@ -2664,20 +4059,51 @@
         <v>1832500</v>
       </c>
       <c r="J56" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-1916693</v>
       </c>
       <c r="K56" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-1729615</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M56" s="15">
+        <v>682906</v>
+      </c>
+      <c r="N56">
+        <v>5040</v>
+      </c>
+      <c r="O56">
+        <v>3000</v>
+      </c>
+      <c r="P56">
+        <v>926</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="S56">
+        <f>1800000+S55</f>
+        <v>1832500</v>
+      </c>
+      <c r="T56" s="1">
+        <f t="shared" si="15"/>
+        <v>-1233787</v>
+      </c>
+      <c r="U56" s="1">
+        <f t="shared" si="17"/>
+        <v>1271803</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="B57">
@@ -2699,27 +4125,51 @@
         <v>0</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J57" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-84193</v>
       </c>
       <c r="K57" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-1813808</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M57" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M57" s="15">
+        <v>699979</v>
+      </c>
+      <c r="N57">
+        <v>5040</v>
+      </c>
+      <c r="O57">
+        <v>3000</v>
+      </c>
+      <c r="P57">
+        <v>926</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T57" s="1">
+        <f t="shared" si="15"/>
+        <v>615786</v>
+      </c>
+      <c r="U57" s="1">
+        <f t="shared" si="17"/>
+        <v>1887589</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="B58">
@@ -2741,21 +4191,48 @@
         <v>0</v>
       </c>
       <c r="H58" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J58" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-84193</v>
       </c>
       <c r="K58" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1898001</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M58" s="15">
+        <v>717479</v>
+      </c>
+      <c r="N58">
+        <v>5040</v>
+      </c>
+      <c r="O58">
+        <v>3000</v>
+      </c>
+      <c r="P58">
+        <v>926</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+      <c r="R58" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T58" s="1">
+        <f t="shared" si="15"/>
+        <v>633286</v>
+      </c>
+      <c r="U58" s="11">
+        <f t="shared" ref="U58:U61" si="18">U57+T58</f>
+        <v>2520875</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="B59">
@@ -2777,21 +4254,48 @@
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>-84193</v>
       </c>
       <c r="K59" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1982194</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M59" s="15">
+        <v>735416</v>
+      </c>
+      <c r="N59">
+        <v>5040</v>
+      </c>
+      <c r="O59">
+        <v>3000</v>
+      </c>
+      <c r="P59">
+        <v>926</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+      <c r="R59" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T59" s="1">
+        <f t="shared" si="15"/>
+        <v>651223</v>
+      </c>
+      <c r="U59" s="11">
+        <f t="shared" si="18"/>
+        <v>3172098</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="B60">
@@ -2813,7 +4317,7 @@
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J60">
@@ -2821,13 +4325,40 @@
         <v>-84193</v>
       </c>
       <c r="K60" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2066387</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M60" s="15">
+        <v>753801</v>
+      </c>
+      <c r="N60">
+        <v>5040</v>
+      </c>
+      <c r="O60">
+        <v>3000</v>
+      </c>
+      <c r="P60">
+        <v>926</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T60">
+        <f t="shared" ref="T60:T118" si="19">M60-N60-O60-P60-Q60-R60</f>
+        <v>669608</v>
+      </c>
+      <c r="U60" s="11">
+        <f t="shared" si="18"/>
+        <v>3841706</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="B61">
@@ -2849,7 +4380,7 @@
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
       <c r="J61">
@@ -2857,8 +4388,35 @@
         <v>-84193</v>
       </c>
       <c r="K61" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2150580</v>
+      </c>
+      <c r="M61" s="15">
+        <v>772646</v>
+      </c>
+      <c r="N61">
+        <v>5040</v>
+      </c>
+      <c r="O61">
+        <v>3000</v>
+      </c>
+      <c r="P61">
+        <v>926</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
+      </c>
+      <c r="R61" s="1">
+        <f t="shared" si="13"/>
+        <v>75227</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="19"/>
+        <v>688453</v>
+      </c>
+      <c r="U61" s="11">
+        <f t="shared" si="18"/>
+        <v>4530159</v>
       </c>
     </row>
   </sheetData>
@@ -2874,9 +4432,9 @@
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2887,7 +4445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2898,7 +4456,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -2910,7 +4468,7 @@
         <v>184500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A61" si="0">A3+1</f>
         <v>2</v>
@@ -2922,7 +4480,7 @@
         <v>189113</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2934,7 +4492,7 @@
         <v>193840</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2946,7 +4504,7 @@
         <v>198686</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2958,7 +4516,7 @@
         <v>203653</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2970,7 +4528,7 @@
         <v>208745</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2982,7 +4540,7 @@
         <v>213963</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2994,7 +4552,7 @@
         <v>219313</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3006,7 +4564,7 @@
         <v>224795</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3018,7 +4576,7 @@
         <v>230415</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3030,7 +4588,7 @@
         <v>236176</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3042,7 +4600,7 @@
         <v>242080</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3054,7 +4612,7 @@
         <v>248132</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3066,7 +4624,7 @@
         <v>254335</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3078,7 +4636,7 @@
         <v>260694</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3090,7 +4648,7 @@
         <v>267211</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3102,7 +4660,7 @@
         <v>273891</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3114,7 +4672,7 @@
         <v>280739</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3126,7 +4684,7 @@
         <v>287757</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3138,7 +4696,7 @@
         <v>294951</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3150,7 +4708,7 @@
         <v>302325</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3162,7 +4720,7 @@
         <v>309883</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3174,7 +4732,7 @@
         <v>317630</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3186,7 +4744,7 @@
         <v>325571</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3198,7 +4756,7 @@
         <v>333710</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3210,7 +4768,7 @@
         <v>342053</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3222,7 +4780,7 @@
         <v>350604</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3234,7 +4792,7 @@
         <v>359369</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3246,7 +4804,7 @@
         <v>368353</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3258,7 +4816,7 @@
         <v>377562</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3270,7 +4828,7 @@
         <v>387001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3282,7 +4840,7 @@
         <v>396676</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3294,7 +4852,7 @@
         <v>406593</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3306,7 +4864,7 @@
         <v>416758</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3318,7 +4876,7 @@
         <v>427177</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3330,7 +4888,7 @@
         <v>437856</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3342,7 +4900,7 @@
         <v>448803</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3354,7 +4912,7 @@
         <v>460023</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3366,7 +4924,7 @@
         <v>471523</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3378,7 +4936,7 @@
         <v>483311</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3390,7 +4948,7 @@
         <v>495394</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3402,7 +4960,7 @@
         <v>507779</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3414,7 +4972,7 @@
         <v>520474</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3426,7 +4984,7 @@
         <v>533485</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3438,7 +4996,7 @@
         <v>546823</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3450,7 +5008,7 @@
         <v>560493</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3462,7 +5020,7 @@
         <v>574505</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3474,7 +5032,7 @@
         <v>588868</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3486,7 +5044,7 @@
         <v>603590</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3498,7 +5056,7 @@
         <v>618680</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -3510,7 +5068,7 @@
         <v>634147</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -3522,7 +5080,7 @@
         <v>650000</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -3534,7 +5092,7 @@
         <v>666250</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -3546,7 +5104,7 @@
         <v>682906</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -3558,7 +5116,7 @@
         <v>699979</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -3570,7 +5128,7 @@
         <v>717479</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -3582,7 +5140,7 @@
         <v>735416</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -3594,7 +5152,7 @@
         <v>753801</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>

</xml_diff>

<commit_message>
Update case 1 and 2
corrected retirement and cancer cost.
</commit_message>
<xml_diff>
--- a/fc/Case1&2.xlsx
+++ b/fc/Case1&2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woongjin/Desktop/Projects/InsuranceGame/fc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\GoI\InsuranceGame\fc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E473FE53-E41B-5841-82FC-D308FAADBA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0648C697-8738-47B3-9CFB-B6F41273EF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23880" yWindow="500" windowWidth="23880" windowHeight="16180" xr2:uid="{93EEACCD-8AF9-48DF-BEAB-81301AC67219}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7360" xr2:uid="{93EEACCD-8AF9-48DF-BEAB-81301AC67219}"/>
   </bookViews>
   <sheets>
     <sheet name="Case_1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>step</t>
   </si>
@@ -110,6 +108,9 @@
   </si>
   <si>
     <t>Not Retired</t>
+  </si>
+  <si>
+    <t>&lt;--end</t>
   </si>
 </sst>
 </file>
@@ -566,20 +567,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AEF988-3009-472E-9717-6E6A120C3C2F}">
   <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="64" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q51" sqref="Q51"/>
+      <selection pane="topRight" activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -638,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -664,7 +669,7 @@
       </c>
       <c r="O2" s="16"/>
       <c r="P2" s="16">
-        <f>N2-S2-T2-U2-V2-W2</f>
+        <f t="shared" ref="P2:P31" si="0">N2-S2-T2-U2-V2-W2</f>
         <v>180000</v>
       </c>
       <c r="Q2" s="16">
@@ -677,7 +682,7 @@
       <c r="V2" s="16"/>
       <c r="W2" s="16"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>1</v>
@@ -692,7 +697,7 @@
         <v>5040</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J61" si="0">C3-D3-E3-F3-G3-H3</f>
+        <f t="shared" ref="J3:J61" si="1">C3-D3-E3-F3-G3-H3</f>
         <v>179460</v>
       </c>
       <c r="K3">
@@ -708,11 +713,11 @@
       </c>
       <c r="O3" s="16"/>
       <c r="P3" s="16">
-        <f>N3-S3-T3-U3-V3-W3</f>
+        <f t="shared" si="0"/>
         <v>179460</v>
       </c>
       <c r="Q3" s="16">
-        <f>Q2+P3</f>
+        <f t="shared" ref="Q3:Q41" si="2">Q2+P3</f>
         <v>359460</v>
       </c>
       <c r="S3" s="16">
@@ -723,9 +728,9 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A61" si="1">A3+1</f>
+        <f t="shared" ref="A4:A61" si="3">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -741,15 +746,15 @@
         <v>3000</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>181073</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K61" si="2">K3+J4</f>
+        <f t="shared" ref="K4:K61" si="4">K3+J4</f>
         <v>540533</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L36" si="3">L3+1</f>
+        <f t="shared" ref="L4:L36" si="5">L3+1</f>
         <v>2</v>
       </c>
       <c r="N4" s="16">
@@ -757,11 +762,11 @@
       </c>
       <c r="O4" s="16"/>
       <c r="P4" s="16">
-        <f>N4-S4-T4-U4-V4-W4</f>
+        <f t="shared" si="0"/>
         <v>181073</v>
       </c>
       <c r="Q4" s="16">
-        <f>Q3+P4</f>
+        <f t="shared" si="2"/>
         <v>540533</v>
       </c>
       <c r="S4" s="16">
@@ -774,9 +779,9 @@
       <c r="V4" s="16"/>
       <c r="W4" s="16"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B5">
@@ -792,15 +797,15 @@
         <v>3000</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>185800</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>726333</v>
       </c>
       <c r="L5" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="N5" s="16">
@@ -808,11 +813,11 @@
       </c>
       <c r="O5" s="16"/>
       <c r="P5" s="16">
-        <f>N5-S5-T5-U5-V5-W5</f>
+        <f t="shared" si="0"/>
         <v>185800</v>
       </c>
       <c r="Q5" s="16">
-        <f>Q4+P5</f>
+        <f t="shared" si="2"/>
         <v>726333</v>
       </c>
       <c r="S5" s="16">
@@ -825,9 +830,9 @@
       <c r="V5" s="16"/>
       <c r="W5" s="16"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B6">
@@ -846,29 +851,29 @@
         <v>926</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>189720</v>
       </c>
       <c r="K6">
+        <f t="shared" si="4"/>
+        <v>916053</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N6" s="16">
+        <v>198686</v>
+      </c>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16">
+        <f t="shared" si="0"/>
+        <v>189720</v>
+      </c>
+      <c r="Q6" s="16">
         <f t="shared" si="2"/>
         <v>916053</v>
       </c>
-      <c r="L6" s="6">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="N6" s="16">
-        <v>198686</v>
-      </c>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16">
-        <f>N6-S6-T6-U6-V6-W6</f>
-        <v>189720</v>
-      </c>
-      <c r="Q6" s="16">
-        <f>Q5+P6</f>
-        <v>916053</v>
-      </c>
       <c r="S6" s="16">
         <v>5040</v>
       </c>
@@ -881,9 +886,9 @@
       <c r="V6" s="16"/>
       <c r="W6" s="16"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B7">
@@ -905,29 +910,29 @@
         <v>18000</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>176687</v>
       </c>
       <c r="K7">
+        <f t="shared" si="4"/>
+        <v>1092740</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="N7" s="16">
+        <v>203653</v>
+      </c>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16">
+        <f t="shared" si="0"/>
+        <v>176687</v>
+      </c>
+      <c r="Q7" s="16">
         <f t="shared" si="2"/>
         <v>1092740</v>
       </c>
-      <c r="L7" s="7">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="N7" s="16">
-        <v>203653</v>
-      </c>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16">
-        <f>N7-S7-T7-U7-V7-W7</f>
-        <v>176687</v>
-      </c>
-      <c r="Q7" s="16">
-        <f>Q6+P7</f>
-        <v>1092740</v>
-      </c>
       <c r="S7" s="16">
         <v>5040</v>
       </c>
@@ -942,9 +947,9 @@
       </c>
       <c r="W7" s="16"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B8">
@@ -966,29 +971,29 @@
         <v>18000</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>181779</v>
       </c>
       <c r="K8">
+        <f t="shared" si="4"/>
+        <v>1274519</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N8" s="16">
+        <v>208745</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16">
+        <f t="shared" si="0"/>
+        <v>181779</v>
+      </c>
+      <c r="Q8" s="16">
         <f t="shared" si="2"/>
         <v>1274519</v>
       </c>
-      <c r="L8" s="8">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="N8" s="16">
-        <v>208745</v>
-      </c>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16">
-        <f>N8-S8-T8-U8-V8-W8</f>
-        <v>181779</v>
-      </c>
-      <c r="Q8" s="16">
-        <f>Q7+P8</f>
-        <v>1274519</v>
-      </c>
       <c r="S8" s="16">
         <v>5040</v>
       </c>
@@ -1003,9 +1008,9 @@
       </c>
       <c r="W8" s="16"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B9">
@@ -1027,29 +1032,29 @@
         <v>18000</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>186997</v>
       </c>
       <c r="K9">
+        <f t="shared" si="4"/>
+        <v>1461516</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="N9" s="16">
+        <v>213963</v>
+      </c>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16">
+        <f t="shared" si="0"/>
+        <v>186997</v>
+      </c>
+      <c r="Q9" s="16">
         <f t="shared" si="2"/>
         <v>1461516</v>
       </c>
-      <c r="L9" s="3">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="N9" s="16">
-        <v>213963</v>
-      </c>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16">
-        <f>N9-S9-T9-U9-V9-W9</f>
-        <v>186997</v>
-      </c>
-      <c r="Q9" s="16">
-        <f>Q8+P9</f>
-        <v>1461516</v>
-      </c>
       <c r="S9" s="16">
         <v>5040</v>
       </c>
@@ -1064,9 +1069,9 @@
       </c>
       <c r="W9" s="16"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B10">
@@ -1088,29 +1093,29 @@
         <v>18000</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>192347</v>
       </c>
       <c r="K10">
+        <f t="shared" si="4"/>
+        <v>1653863</v>
+      </c>
+      <c r="L10" s="9">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="N10" s="16">
+        <v>219313</v>
+      </c>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16">
+        <f t="shared" si="0"/>
+        <v>192347</v>
+      </c>
+      <c r="Q10" s="16">
         <f t="shared" si="2"/>
         <v>1653863</v>
       </c>
-      <c r="L10" s="9">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="N10" s="16">
-        <v>219313</v>
-      </c>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16">
-        <f>N10-S10-T10-U10-V10-W10</f>
-        <v>192347</v>
-      </c>
-      <c r="Q10" s="16">
-        <f>Q9+P10</f>
-        <v>1653863</v>
-      </c>
       <c r="S10" s="16">
         <v>5040</v>
       </c>
@@ -1125,9 +1130,9 @@
       </c>
       <c r="W10" s="16"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B11">
@@ -1149,29 +1154,29 @@
         <v>18000</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>197829</v>
       </c>
       <c r="K11">
+        <f t="shared" si="4"/>
+        <v>1851692</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="N11" s="16">
+        <v>224795</v>
+      </c>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16">
+        <f t="shared" si="0"/>
+        <v>197829</v>
+      </c>
+      <c r="Q11" s="16">
         <f t="shared" si="2"/>
         <v>1851692</v>
       </c>
-      <c r="L11" s="5">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="N11" s="16">
-        <v>224795</v>
-      </c>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16">
-        <f>N11-S11-T11-U11-V11-W11</f>
-        <v>197829</v>
-      </c>
-      <c r="Q11" s="16">
-        <f>Q10+P11</f>
-        <v>1851692</v>
-      </c>
       <c r="S11" s="16">
         <v>5040</v>
       </c>
@@ -1186,9 +1191,9 @@
       </c>
       <c r="W11" s="16"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B12">
@@ -1210,29 +1215,29 @@
         <v>18000</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>203449</v>
       </c>
       <c r="K12">
+        <f t="shared" si="4"/>
+        <v>2055141</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="N12" s="16">
+        <v>230415</v>
+      </c>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16">
+        <f t="shared" si="0"/>
+        <v>203449</v>
+      </c>
+      <c r="Q12" s="16">
         <f t="shared" si="2"/>
         <v>2055141</v>
       </c>
-      <c r="L12" s="6">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="N12" s="16">
-        <v>230415</v>
-      </c>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16">
-        <f>N12-S12-T12-U12-V12-W12</f>
-        <v>203449</v>
-      </c>
-      <c r="Q12" s="16">
-        <f>Q11+P12</f>
-        <v>2055141</v>
-      </c>
       <c r="S12" s="16">
         <v>5040</v>
       </c>
@@ -1247,9 +1252,9 @@
       </c>
       <c r="W12" s="16"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B13">
@@ -1271,29 +1276,29 @@
         <v>18000</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>209210</v>
       </c>
       <c r="K13">
+        <f t="shared" si="4"/>
+        <v>2264351</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="N13" s="16">
+        <v>236176</v>
+      </c>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16">
+        <f t="shared" si="0"/>
+        <v>209210</v>
+      </c>
+      <c r="Q13" s="16">
         <f t="shared" si="2"/>
         <v>2264351</v>
       </c>
-      <c r="L13" s="7">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="N13" s="16">
-        <v>236176</v>
-      </c>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16">
-        <f>N13-S13-T13-U13-V13-W13</f>
-        <v>209210</v>
-      </c>
-      <c r="Q13" s="16">
-        <f>Q12+P13</f>
-        <v>2264351</v>
-      </c>
       <c r="S13" s="16">
         <v>5040</v>
       </c>
@@ -1308,9 +1313,9 @@
       </c>
       <c r="W13" s="16"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B14">
@@ -1332,29 +1337,29 @@
         <v>18000</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>215114</v>
       </c>
       <c r="K14">
+        <f t="shared" si="4"/>
+        <v>2479465</v>
+      </c>
+      <c r="L14" s="8">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="N14" s="16">
+        <v>242080</v>
+      </c>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16">
+        <f t="shared" si="0"/>
+        <v>215114</v>
+      </c>
+      <c r="Q14" s="16">
         <f t="shared" si="2"/>
         <v>2479465</v>
       </c>
-      <c r="L14" s="8">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="N14" s="16">
-        <v>242080</v>
-      </c>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16">
-        <f>N14-S14-T14-U14-V14-W14</f>
-        <v>215114</v>
-      </c>
-      <c r="Q14" s="16">
-        <f>Q13+P14</f>
-        <v>2479465</v>
-      </c>
       <c r="S14" s="16">
         <v>5040</v>
       </c>
@@ -1369,9 +1374,9 @@
       </c>
       <c r="W14" s="16"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B15">
@@ -1393,29 +1398,29 @@
         <v>18000</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>221166</v>
       </c>
       <c r="K15">
+        <f t="shared" si="4"/>
+        <v>2700631</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="N15" s="16">
+        <v>248132</v>
+      </c>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16">
+        <f t="shared" si="0"/>
+        <v>221166</v>
+      </c>
+      <c r="Q15" s="16">
         <f t="shared" si="2"/>
         <v>2700631</v>
       </c>
-      <c r="L15" s="3">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="N15" s="16">
-        <v>248132</v>
-      </c>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16">
-        <f>N15-S15-T15-U15-V15-W15</f>
-        <v>221166</v>
-      </c>
-      <c r="Q15" s="16">
-        <f>Q14+P15</f>
-        <v>2700631</v>
-      </c>
       <c r="S15" s="16">
         <v>5040</v>
       </c>
@@ -1430,9 +1435,9 @@
       </c>
       <c r="W15" s="16"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B16">
@@ -1454,29 +1459,29 @@
         <v>18000</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>227369</v>
       </c>
       <c r="K16">
+        <f t="shared" si="4"/>
+        <v>2928000</v>
+      </c>
+      <c r="L16" s="9">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="N16" s="16">
+        <v>254335</v>
+      </c>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16">
+        <f t="shared" si="0"/>
+        <v>227369</v>
+      </c>
+      <c r="Q16" s="16">
         <f t="shared" si="2"/>
         <v>2928000</v>
       </c>
-      <c r="L16" s="9">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="N16" s="16">
-        <v>254335</v>
-      </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16">
-        <f>N16-S16-T16-U16-V16-W16</f>
-        <v>227369</v>
-      </c>
-      <c r="Q16" s="16">
-        <f>Q15+P16</f>
-        <v>2928000</v>
-      </c>
       <c r="S16" s="16">
         <v>5040</v>
       </c>
@@ -1491,9 +1496,9 @@
       </c>
       <c r="W16" s="16"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B17">
@@ -1515,29 +1520,29 @@
         <v>18000</v>
       </c>
       <c r="J17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>233728</v>
       </c>
       <c r="K17">
+        <f t="shared" si="4"/>
+        <v>3161728</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="N17" s="16">
+        <v>260694</v>
+      </c>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16">
+        <f t="shared" si="0"/>
+        <v>233728</v>
+      </c>
+      <c r="Q17" s="16">
         <f t="shared" si="2"/>
         <v>3161728</v>
       </c>
-      <c r="L17" s="5">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="N17" s="16">
-        <v>260694</v>
-      </c>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16">
-        <f>N17-S17-T17-U17-V17-W17</f>
-        <v>233728</v>
-      </c>
-      <c r="Q17" s="16">
-        <f>Q16+P17</f>
-        <v>3161728</v>
-      </c>
       <c r="S17" s="16">
         <v>5040</v>
       </c>
@@ -1552,9 +1557,9 @@
       </c>
       <c r="W17" s="16"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="B18">
@@ -1576,29 +1581,29 @@
         <v>18000</v>
       </c>
       <c r="J18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>240245</v>
       </c>
       <c r="K18">
+        <f t="shared" si="4"/>
+        <v>3401973</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="N18" s="16">
+        <v>267211</v>
+      </c>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16">
+        <f t="shared" si="0"/>
+        <v>240245</v>
+      </c>
+      <c r="Q18" s="16">
         <f t="shared" si="2"/>
         <v>3401973</v>
       </c>
-      <c r="L18" s="6">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="N18" s="16">
-        <v>267211</v>
-      </c>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16">
-        <f>N18-S18-T18-U18-V18-W18</f>
-        <v>240245</v>
-      </c>
-      <c r="Q18" s="16">
-        <f>Q17+P18</f>
-        <v>3401973</v>
-      </c>
       <c r="S18" s="16">
         <v>5040</v>
       </c>
@@ -1613,9 +1618,9 @@
       </c>
       <c r="W18" s="16"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B19">
@@ -1637,29 +1642,29 @@
         <v>18000</v>
       </c>
       <c r="J19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>246925</v>
       </c>
       <c r="K19">
+        <f t="shared" si="4"/>
+        <v>3648898</v>
+      </c>
+      <c r="L19" s="7">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="N19" s="16">
+        <v>273891</v>
+      </c>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16">
+        <f t="shared" si="0"/>
+        <v>246925</v>
+      </c>
+      <c r="Q19" s="16">
         <f t="shared" si="2"/>
         <v>3648898</v>
       </c>
-      <c r="L19" s="7">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="N19" s="16">
-        <v>273891</v>
-      </c>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16">
-        <f>N19-S19-T19-U19-V19-W19</f>
-        <v>246925</v>
-      </c>
-      <c r="Q19" s="16">
-        <f>Q18+P19</f>
-        <v>3648898</v>
-      </c>
       <c r="S19" s="16">
         <v>5040</v>
       </c>
@@ -1674,9 +1679,9 @@
       </c>
       <c r="W19" s="16"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B20">
@@ -1701,29 +1706,29 @@
         <v>28074</v>
       </c>
       <c r="J20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>225699</v>
       </c>
       <c r="K20">
+        <f t="shared" si="4"/>
+        <v>3874597</v>
+      </c>
+      <c r="L20" s="8">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="N20" s="16">
+        <v>280739</v>
+      </c>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16">
+        <f t="shared" si="0"/>
+        <v>225699</v>
+      </c>
+      <c r="Q20" s="16">
         <f t="shared" si="2"/>
         <v>3874597</v>
       </c>
-      <c r="L20" s="8">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="N20" s="16">
-        <v>280739</v>
-      </c>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16">
-        <f>N20-S20-T20-U20-V20-W20</f>
-        <v>225699</v>
-      </c>
-      <c r="Q20" s="16">
-        <f>Q19+P20</f>
-        <v>3874597</v>
-      </c>
       <c r="S20" s="16">
         <v>5040</v>
       </c>
@@ -1740,9 +1745,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B21">
@@ -1767,29 +1772,29 @@
         <v>28074</v>
       </c>
       <c r="J21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>232717</v>
       </c>
       <c r="K21">
+        <f t="shared" si="4"/>
+        <v>4107314</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="N21" s="16">
+        <v>287757</v>
+      </c>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16">
+        <f t="shared" si="0"/>
+        <v>232717</v>
+      </c>
+      <c r="Q21" s="16">
         <f t="shared" si="2"/>
         <v>4107314</v>
       </c>
-      <c r="L21" s="3">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="N21" s="16">
-        <v>287757</v>
-      </c>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16">
-        <f>N21-S21-T21-U21-V21-W21</f>
-        <v>232717</v>
-      </c>
-      <c r="Q21" s="16">
-        <f>Q20+P21</f>
-        <v>4107314</v>
-      </c>
       <c r="S21" s="16">
         <v>5040</v>
       </c>
@@ -1806,9 +1811,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B22">
@@ -1833,29 +1838,29 @@
         <v>28074</v>
       </c>
       <c r="J22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>239911</v>
       </c>
       <c r="K22">
+        <f t="shared" si="4"/>
+        <v>4347225</v>
+      </c>
+      <c r="L22" s="9">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="N22" s="16">
+        <v>294951</v>
+      </c>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16">
+        <f t="shared" si="0"/>
+        <v>239911</v>
+      </c>
+      <c r="Q22" s="16">
         <f t="shared" si="2"/>
         <v>4347225</v>
       </c>
-      <c r="L22" s="9">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="N22" s="16">
-        <v>294951</v>
-      </c>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16">
-        <f>N22-S22-T22-U22-V22-W22</f>
-        <v>239911</v>
-      </c>
-      <c r="Q22" s="16">
-        <f>Q21+P22</f>
-        <v>4347225</v>
-      </c>
       <c r="S22" s="16">
         <v>5040</v>
       </c>
@@ -1872,9 +1877,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B23">
@@ -1899,29 +1904,29 @@
         <v>28074</v>
       </c>
       <c r="J23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>247285</v>
       </c>
       <c r="K23">
+        <f t="shared" si="4"/>
+        <v>4594510</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="N23" s="16">
+        <v>302325</v>
+      </c>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16">
+        <f t="shared" si="0"/>
+        <v>247285</v>
+      </c>
+      <c r="Q23" s="16">
         <f t="shared" si="2"/>
         <v>4594510</v>
       </c>
-      <c r="L23" s="5">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="N23" s="16">
-        <v>302325</v>
-      </c>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16">
-        <f>N23-S23-T23-U23-V23-W23</f>
-        <v>247285</v>
-      </c>
-      <c r="Q23" s="16">
-        <f>Q22+P23</f>
-        <v>4594510</v>
-      </c>
       <c r="S23" s="16">
         <v>5040</v>
       </c>
@@ -1938,9 +1943,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B24">
@@ -1965,29 +1970,29 @@
         <v>28074</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>254843</v>
       </c>
       <c r="K24">
+        <f t="shared" si="4"/>
+        <v>4849353</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="N24" s="16">
+        <v>309883</v>
+      </c>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16">
+        <f t="shared" si="0"/>
+        <v>254843</v>
+      </c>
+      <c r="Q24" s="16">
         <f t="shared" si="2"/>
         <v>4849353</v>
       </c>
-      <c r="L24" s="6">
-        <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="N24" s="16">
-        <v>309883</v>
-      </c>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16">
-        <f>N24-S24-T24-U24-V24-W24</f>
-        <v>254843</v>
-      </c>
-      <c r="Q24" s="16">
-        <f>Q23+P24</f>
-        <v>4849353</v>
-      </c>
       <c r="S24" s="16">
         <v>5040</v>
       </c>
@@ -2004,9 +2009,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B25">
@@ -2031,29 +2036,29 @@
         <v>28074</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>262590</v>
       </c>
       <c r="K25">
+        <f t="shared" si="4"/>
+        <v>5111943</v>
+      </c>
+      <c r="L25" s="7">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="N25" s="16">
+        <v>317630</v>
+      </c>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16">
+        <f t="shared" si="0"/>
+        <v>262590</v>
+      </c>
+      <c r="Q25" s="16">
         <f t="shared" si="2"/>
         <v>5111943</v>
       </c>
-      <c r="L25" s="7">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="N25" s="16">
-        <v>317630</v>
-      </c>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16">
-        <f>N25-S25-T25-U25-V25-W25</f>
-        <v>262590</v>
-      </c>
-      <c r="Q25" s="16">
-        <f>Q24+P25</f>
-        <v>5111943</v>
-      </c>
       <c r="S25" s="16">
         <v>5040</v>
       </c>
@@ -2070,9 +2075,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B26">
@@ -2097,29 +2102,29 @@
         <v>28074</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>270531</v>
       </c>
       <c r="K26">
+        <f t="shared" si="4"/>
+        <v>5382474</v>
+      </c>
+      <c r="L26" s="8">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="N26" s="16">
+        <v>325571</v>
+      </c>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16">
+        <f t="shared" si="0"/>
+        <v>270531</v>
+      </c>
+      <c r="Q26" s="16">
         <f t="shared" si="2"/>
         <v>5382474</v>
       </c>
-      <c r="L26" s="8">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="N26" s="16">
-        <v>325571</v>
-      </c>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16">
-        <f>N26-S26-T26-U26-V26-W26</f>
-        <v>270531</v>
-      </c>
-      <c r="Q26" s="16">
-        <f>Q25+P26</f>
-        <v>5382474</v>
-      </c>
       <c r="S26" s="16">
         <v>5040</v>
       </c>
@@ -2136,9 +2141,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B27">
@@ -2163,29 +2168,29 @@
         <v>28074</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>278670</v>
       </c>
       <c r="K27">
+        <f t="shared" si="4"/>
+        <v>5661144</v>
+      </c>
+      <c r="L27" s="3">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="N27" s="16">
+        <v>333710</v>
+      </c>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16">
+        <f t="shared" si="0"/>
+        <v>278670</v>
+      </c>
+      <c r="Q27" s="16">
         <f t="shared" si="2"/>
         <v>5661144</v>
       </c>
-      <c r="L27" s="3">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="N27" s="16">
-        <v>333710</v>
-      </c>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16">
-        <f>N27-S27-T27-U27-V27-W27</f>
-        <v>278670</v>
-      </c>
-      <c r="Q27" s="16">
-        <f>Q26+P27</f>
-        <v>5661144</v>
-      </c>
       <c r="S27" s="16">
         <v>5040</v>
       </c>
@@ -2202,9 +2207,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B28">
@@ -2229,29 +2234,29 @@
         <v>28074</v>
       </c>
       <c r="J28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>287013</v>
       </c>
       <c r="K28">
+        <f t="shared" si="4"/>
+        <v>5948157</v>
+      </c>
+      <c r="L28" s="9">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="N28" s="16">
+        <v>342053</v>
+      </c>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16">
+        <f t="shared" si="0"/>
+        <v>287013</v>
+      </c>
+      <c r="Q28" s="16">
         <f t="shared" si="2"/>
         <v>5948157</v>
       </c>
-      <c r="L28" s="9">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="N28" s="16">
-        <v>342053</v>
-      </c>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16">
-        <f>N28-S28-T28-U28-V28-W28</f>
-        <v>287013</v>
-      </c>
-      <c r="Q28" s="16">
-        <f>Q27+P28</f>
-        <v>5948157</v>
-      </c>
       <c r="S28" s="16">
         <v>5040</v>
       </c>
@@ -2268,9 +2273,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B29">
@@ -2295,29 +2300,29 @@
         <v>28074</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>295564</v>
       </c>
       <c r="K29">
+        <f t="shared" si="4"/>
+        <v>6243721</v>
+      </c>
+      <c r="L29" s="5">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="N29" s="16">
+        <v>350604</v>
+      </c>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16">
+        <f t="shared" si="0"/>
+        <v>295564</v>
+      </c>
+      <c r="Q29" s="16">
         <f t="shared" si="2"/>
         <v>6243721</v>
       </c>
-      <c r="L29" s="5">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="N29" s="16">
-        <v>350604</v>
-      </c>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16">
-        <f>N29-S29-T29-U29-V29-W29</f>
-        <v>295564</v>
-      </c>
-      <c r="Q29" s="16">
-        <f>Q28+P29</f>
-        <v>6243721</v>
-      </c>
       <c r="S29" s="16">
         <v>5040</v>
       </c>
@@ -2334,9 +2339,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B30">
@@ -2361,29 +2366,29 @@
         <v>28074</v>
       </c>
       <c r="J30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>304329</v>
       </c>
       <c r="K30">
+        <f t="shared" si="4"/>
+        <v>6548050</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="N30" s="16">
+        <v>359369</v>
+      </c>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16">
+        <f t="shared" si="0"/>
+        <v>304329</v>
+      </c>
+      <c r="Q30" s="16">
         <f t="shared" si="2"/>
         <v>6548050</v>
       </c>
-      <c r="L30" s="6">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="N30" s="16">
-        <v>359369</v>
-      </c>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16">
-        <f>N30-S30-T30-U30-V30-W30</f>
-        <v>304329</v>
-      </c>
-      <c r="Q30" s="16">
-        <f>Q29+P30</f>
-        <v>6548050</v>
-      </c>
       <c r="S30" s="16">
         <v>5040</v>
       </c>
@@ -2400,9 +2405,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="B31">
@@ -2427,29 +2432,29 @@
         <v>28074</v>
       </c>
       <c r="J31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>313313</v>
       </c>
       <c r="K31">
+        <f t="shared" si="4"/>
+        <v>6861363</v>
+      </c>
+      <c r="L31" s="7">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="N31" s="16">
+        <v>368353</v>
+      </c>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16">
+        <f t="shared" si="0"/>
+        <v>313313</v>
+      </c>
+      <c r="Q31" s="16">
         <f t="shared" si="2"/>
         <v>6861363</v>
       </c>
-      <c r="L31" s="7">
-        <f t="shared" si="3"/>
-        <v>29</v>
-      </c>
-      <c r="N31" s="16">
-        <v>368353</v>
-      </c>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16">
-        <f>N31-S31-T31-U31-V31-W31</f>
-        <v>313313</v>
-      </c>
-      <c r="Q31" s="16">
-        <f>Q30+P31</f>
-        <v>6861363</v>
-      </c>
       <c r="S31" s="16">
         <v>5040</v>
       </c>
@@ -2466,9 +2471,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B32">
@@ -2497,11 +2502,11 @@
         <v>830535</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7691898</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="N32" s="16">
@@ -2513,7 +2518,7 @@
         <v>830535</v>
       </c>
       <c r="Q32" s="16">
-        <f>Q31+P32</f>
+        <f t="shared" si="2"/>
         <v>7691898</v>
       </c>
       <c r="S32" s="16">
@@ -2532,9 +2537,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B33">
@@ -2563,11 +2568,11 @@
         <v>349961</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8041859</v>
       </c>
       <c r="L33" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="N33" s="16">
@@ -2579,7 +2584,7 @@
         <v>349961</v>
       </c>
       <c r="Q33" s="16">
-        <f>Q32+P33</f>
+        <f t="shared" si="2"/>
         <v>8041859</v>
       </c>
       <c r="S33" s="16">
@@ -2598,9 +2603,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B34">
@@ -2625,15 +2630,15 @@
         <v>28074</v>
       </c>
       <c r="J34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>359636</v>
       </c>
       <c r="K34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8401495</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="N34" s="16">
@@ -2645,7 +2650,7 @@
         <v>359636</v>
       </c>
       <c r="Q34" s="16">
-        <f>Q33+P34</f>
+        <f t="shared" si="2"/>
         <v>8401495</v>
       </c>
       <c r="S34" s="16">
@@ -2664,9 +2669,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B35">
@@ -2691,15 +2696,15 @@
         <v>28074</v>
       </c>
       <c r="J35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>369553</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8771048</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="N35" s="16">
@@ -2711,7 +2716,7 @@
         <v>369553</v>
       </c>
       <c r="Q35" s="16">
-        <f>Q34+P35</f>
+        <f t="shared" si="2"/>
         <v>8771048</v>
       </c>
       <c r="S35" s="16">
@@ -2730,9 +2735,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B36">
@@ -2757,15 +2762,15 @@
         <v>28074</v>
       </c>
       <c r="J36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>379718</v>
       </c>
       <c r="K36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9150766</v>
       </c>
       <c r="L36" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="N36" s="16">
@@ -2777,7 +2782,7 @@
         <v>379718</v>
       </c>
       <c r="Q36" s="16">
-        <f>Q35+P36</f>
+        <f t="shared" si="2"/>
         <v>9150766</v>
       </c>
       <c r="S36" s="16">
@@ -2796,9 +2801,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B37">
@@ -2823,11 +2828,11 @@
         <v>28074</v>
       </c>
       <c r="J37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-37040</v>
       </c>
       <c r="K37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9113726</v>
       </c>
       <c r="L37" s="10" t="s">
@@ -2842,7 +2847,7 @@
         <v>-37040</v>
       </c>
       <c r="Q37" s="16">
-        <f>Q36+P37</f>
+        <f t="shared" si="2"/>
         <v>9113726</v>
       </c>
       <c r="S37" s="16">
@@ -2861,9 +2866,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B38">
@@ -2895,7 +2900,7 @@
         <v>-337040</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8776686</v>
       </c>
       <c r="L38" s="10" t="s">
@@ -2912,7 +2917,7 @@
         <v>-337040</v>
       </c>
       <c r="Q38" s="16">
-        <f>Q37+P38</f>
+        <f t="shared" si="2"/>
         <v>8776686</v>
       </c>
       <c r="S38" s="16">
@@ -2931,9 +2936,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="B39">
@@ -2965,7 +2970,7 @@
         <v>-337040</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8439646</v>
       </c>
       <c r="L39" s="10" t="s">
@@ -2982,7 +2987,7 @@
         <v>-337040</v>
       </c>
       <c r="Q39" s="16">
-        <f>Q38+P39</f>
+        <f t="shared" si="2"/>
         <v>8439646</v>
       </c>
       <c r="S39" s="16">
@@ -3001,9 +3006,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="B40">
@@ -3028,11 +3033,11 @@
         <v>28074</v>
       </c>
       <c r="J40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-37040</v>
       </c>
       <c r="K40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8402606</v>
       </c>
       <c r="L40" s="10" t="s">
@@ -3047,7 +3052,7 @@
         <v>-37040</v>
       </c>
       <c r="Q40" s="16">
-        <f>Q39+P40</f>
+        <f t="shared" si="2"/>
         <v>8402606</v>
       </c>
       <c r="S40" s="16">
@@ -3066,9 +3071,9 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="B41">
@@ -3090,15 +3095,15 @@
         <v>0</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" ref="H41:H42" si="4">28074+ROUNDUP(471523*10%, 0)</f>
+        <f t="shared" ref="H41:H42" si="6">28074+ROUNDUP(471523*10%, 0)</f>
         <v>75227</v>
       </c>
       <c r="J41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-84193</v>
       </c>
       <c r="K41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8318413</v>
       </c>
       <c r="L41" s="10" t="s">
@@ -3113,7 +3118,7 @@
         <v>-84193</v>
       </c>
       <c r="Q41" s="16">
-        <f>Q40+P41</f>
+        <f t="shared" si="2"/>
         <v>8318413</v>
       </c>
       <c r="S41" s="16">
@@ -3129,13 +3134,13 @@
         <v>0</v>
       </c>
       <c r="W41" s="17">
-        <f t="shared" ref="W41:W42" si="5">28074+ROUNDUP(471523*10%, 0)</f>
+        <f t="shared" ref="W41:W42" si="7">28074+ROUNDUP(471523*10%, 0)</f>
         <v>75227</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="B42">
@@ -3157,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>75227</v>
       </c>
       <c r="I42">
@@ -3183,7 +3188,7 @@
         <v>1663682.6</v>
       </c>
       <c r="P42" s="17">
-        <f>N42-S42-T42-U42-V42-W42-O42</f>
+        <f t="shared" ref="P42:P59" si="8">N42-S42-T42-U42-V42-W42-O42</f>
         <v>-1747875.6</v>
       </c>
       <c r="Q42" s="17">
@@ -3203,13 +3208,13 @@
         <v>0</v>
       </c>
       <c r="W42" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="B43">
@@ -3242,7 +3247,7 @@
         <v>-1588799</v>
       </c>
       <c r="K43" s="1">
-        <f t="shared" ref="K43:K57" si="6">ROUNDDOWN(K42+J43, 0)</f>
+        <f t="shared" ref="K43:K57" si="9">ROUNDDOWN(K42+J43, 0)</f>
         <v>4981738</v>
       </c>
       <c r="L43" s="10" t="s">
@@ -3255,11 +3260,11 @@
         <v>2000000</v>
       </c>
       <c r="P43" s="17">
-        <f>N43-S43-T43-U43-V43-W43-O43</f>
+        <f t="shared" si="8"/>
         <v>-1588799</v>
       </c>
       <c r="Q43" s="17">
-        <f>ROUNDDOWN(Q42+P43, 0)</f>
+        <f t="shared" ref="Q43:Q57" si="10">ROUNDDOWN(Q42+P43, 0)</f>
         <v>4981738</v>
       </c>
       <c r="S43" s="16">
@@ -3279,9 +3284,9 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="B44">
@@ -3303,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" ref="H44:H61" si="7">H43</f>
+        <f t="shared" ref="H44:H61" si="11">H43</f>
         <v>75227</v>
       </c>
       <c r="I44">
@@ -3329,11 +3334,11 @@
         <v>2490869</v>
       </c>
       <c r="P44" s="17">
-        <f>N44-S44-T44-U44-V44-W44-O44</f>
+        <f t="shared" si="8"/>
         <v>-2067283</v>
       </c>
       <c r="Q44" s="17">
-        <f>ROUNDDOWN(Q43+P44, 0)</f>
+        <f t="shared" si="10"/>
         <v>2914455</v>
       </c>
       <c r="S44" s="16">
@@ -3349,13 +3354,13 @@
         <v>0</v>
       </c>
       <c r="W44" s="17">
-        <f t="shared" ref="W44:W61" si="8">W43</f>
+        <f t="shared" ref="W44:W61" si="12">W43</f>
         <v>75227</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="B45">
@@ -3377,18 +3382,18 @@
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="I45">
         <v>1000000</v>
       </c>
       <c r="J45" s="1">
-        <f t="shared" ref="J45:J59" si="9">C45-D45-E45-F45-G45-H45-I45</f>
+        <f t="shared" ref="J45:J59" si="13">C45-D45-E45-F45-G45-H45-I45</f>
         <v>-563719</v>
       </c>
       <c r="K45" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2350736</v>
       </c>
       <c r="L45" s="10" t="s">
@@ -3401,11 +3406,11 @@
         <v>1000000</v>
       </c>
       <c r="P45" s="17">
-        <f>N45-S45-T45-U45-V45-W45-O45</f>
+        <f t="shared" si="8"/>
         <v>-563719</v>
       </c>
       <c r="Q45" s="17">
-        <f>ROUNDDOWN(Q44+P45, 0)</f>
+        <f t="shared" si="10"/>
         <v>2350736</v>
       </c>
       <c r="S45" s="16">
@@ -3421,13 +3426,13 @@
         <v>0</v>
       </c>
       <c r="W45" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="B46" s="12">
@@ -3449,16 +3454,16 @@
         <v>0</v>
       </c>
       <c r="H46" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="I46" s="12"/>
       <c r="J46" s="13">
+        <f t="shared" si="13"/>
+        <v>449292</v>
+      </c>
+      <c r="K46" s="13">
         <f t="shared" si="9"/>
-        <v>449292</v>
-      </c>
-      <c r="K46" s="13">
-        <f t="shared" si="6"/>
         <v>2800028</v>
       </c>
       <c r="L46" s="14" t="s">
@@ -3469,11 +3474,11 @@
       </c>
       <c r="O46" s="18"/>
       <c r="P46" s="19">
-        <f>N46-S46-T46-U46-V46-W46-O46</f>
+        <f t="shared" si="8"/>
         <v>449292</v>
       </c>
       <c r="Q46" s="19">
-        <f>ROUNDDOWN(Q45+P46, 0)</f>
+        <f t="shared" si="10"/>
         <v>2800028</v>
       </c>
       <c r="S46" s="18">
@@ -3489,13 +3494,13 @@
         <v>0</v>
       </c>
       <c r="W46" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="B47">
@@ -3517,15 +3522,15 @@
         <v>0</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J47" s="1">
+        <f t="shared" si="13"/>
+        <v>462630</v>
+      </c>
+      <c r="K47" s="1">
         <f t="shared" si="9"/>
-        <v>462630</v>
-      </c>
-      <c r="K47" s="1">
-        <f t="shared" si="6"/>
         <v>3262658</v>
       </c>
       <c r="L47" s="10" t="s">
@@ -3536,11 +3541,11 @@
       </c>
       <c r="O47" s="16"/>
       <c r="P47" s="17">
-        <f>N47-S47-T47-U47-V47-W47-O47</f>
+        <f t="shared" si="8"/>
         <v>462630</v>
       </c>
       <c r="Q47" s="17">
-        <f>ROUNDDOWN(Q46+P47, 0)</f>
+        <f t="shared" si="10"/>
         <v>3262658</v>
       </c>
       <c r="S47" s="16">
@@ -3556,13 +3561,13 @@
         <v>0</v>
       </c>
       <c r="W47" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="B48">
@@ -3584,15 +3589,15 @@
         <v>0</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J48" s="1">
+        <f t="shared" si="13"/>
+        <v>476300</v>
+      </c>
+      <c r="K48" s="1">
         <f t="shared" si="9"/>
-        <v>476300</v>
-      </c>
-      <c r="K48" s="1">
-        <f t="shared" si="6"/>
         <v>3738958</v>
       </c>
       <c r="L48" s="10" t="s">
@@ -3603,11 +3608,11 @@
       </c>
       <c r="O48" s="16"/>
       <c r="P48" s="17">
-        <f>N48-S48-T48-U48-V48-W48-O48</f>
+        <f t="shared" si="8"/>
         <v>476300</v>
       </c>
       <c r="Q48" s="17">
-        <f>ROUNDDOWN(Q47+P48, 0)</f>
+        <f t="shared" si="10"/>
         <v>3738958</v>
       </c>
       <c r="S48" s="16">
@@ -3623,13 +3628,13 @@
         <v>0</v>
       </c>
       <c r="W48" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="B49">
@@ -3651,18 +3656,18 @@
         <v>0</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="I49">
         <v>1000000</v>
       </c>
       <c r="J49" s="1">
+        <f t="shared" si="13"/>
+        <v>-509688</v>
+      </c>
+      <c r="K49" s="1">
         <f t="shared" si="9"/>
-        <v>-509688</v>
-      </c>
-      <c r="K49" s="1">
-        <f t="shared" si="6"/>
         <v>3229270</v>
       </c>
       <c r="L49" s="10" t="s">
@@ -3675,11 +3680,11 @@
         <v>1000000</v>
       </c>
       <c r="P49" s="17">
-        <f>N49-S49-T49-U49-V49-W49-O49</f>
+        <f t="shared" si="8"/>
         <v>-509688</v>
       </c>
       <c r="Q49" s="17">
-        <f>ROUNDDOWN(Q48+P49, 0)</f>
+        <f t="shared" si="10"/>
         <v>3229270</v>
       </c>
       <c r="S49" s="16">
@@ -3695,13 +3700,13 @@
         <v>0</v>
       </c>
       <c r="W49" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="B50">
@@ -3723,18 +3728,18 @@
         <v>0</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="I50">
         <v>720000</v>
       </c>
       <c r="J50" s="1">
+        <f t="shared" si="13"/>
+        <v>-215325</v>
+      </c>
+      <c r="K50" s="1">
         <f t="shared" si="9"/>
-        <v>-215325</v>
-      </c>
-      <c r="K50" s="1">
-        <f t="shared" si="6"/>
         <v>3013945</v>
       </c>
       <c r="L50" s="10" t="s">
@@ -3747,11 +3752,11 @@
         <v>720000</v>
       </c>
       <c r="P50" s="17">
-        <f>N50-S50-T50-U50-V50-W50-O50</f>
+        <f t="shared" si="8"/>
         <v>-215325</v>
       </c>
       <c r="Q50" s="17">
-        <f>ROUNDDOWN(Q49+P50, 0)</f>
+        <f t="shared" si="10"/>
         <v>3013945</v>
       </c>
       <c r="S50" s="16">
@@ -3767,20 +3772,20 @@
         <v>0</v>
       </c>
       <c r="W50" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="B51">
         <v>60</v>
       </c>
       <c r="C51">
-        <v>603590</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>5040</v>
@@ -3795,16 +3800,16 @@
         <v>0</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J51" s="1">
+        <f t="shared" si="13"/>
+        <v>-84193</v>
+      </c>
+      <c r="K51" s="1">
         <f t="shared" si="9"/>
-        <v>519397</v>
-      </c>
-      <c r="K51" s="1">
-        <f t="shared" si="6"/>
-        <v>3533342</v>
+        <v>2929752</v>
       </c>
       <c r="L51" s="10" t="s">
         <v>22</v>
@@ -3816,11 +3821,11 @@
         <v>603590</v>
       </c>
       <c r="P51" s="1">
-        <f>N51-S51-T51-U51-V51-W51-O51</f>
+        <f t="shared" si="8"/>
         <v>519397</v>
       </c>
       <c r="Q51" s="1">
-        <f>ROUNDDOWN(Q50+P51, 0)</f>
+        <f t="shared" si="10"/>
         <v>3533342</v>
       </c>
       <c r="S51">
@@ -3836,13 +3841,13 @@
         <v>0</v>
       </c>
       <c r="W51" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="B52">
@@ -3864,16 +3869,16 @@
         <v>0</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J52" s="1">
+        <f t="shared" si="13"/>
+        <v>-84193</v>
+      </c>
+      <c r="K52" s="1">
         <f t="shared" si="9"/>
-        <v>-84193</v>
-      </c>
-      <c r="K52" s="1">
-        <f t="shared" si="6"/>
-        <v>3449149</v>
+        <v>2845559</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>20</v>
@@ -3882,11 +3887,11 @@
         <v>618680</v>
       </c>
       <c r="P52" s="1">
-        <f>N52-S52-T52-U52-V52-W52-O52</f>
+        <f t="shared" si="8"/>
         <v>534487</v>
       </c>
       <c r="Q52" s="1">
-        <f>ROUNDDOWN(Q51+P52, 0)</f>
+        <f t="shared" si="10"/>
         <v>4067829</v>
       </c>
       <c r="S52">
@@ -3902,13 +3907,13 @@
         <v>0</v>
       </c>
       <c r="W52" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="B53">
@@ -3930,19 +3935,19 @@
         <v>0</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="I53">
-        <v>1800000</v>
+        <v>720000</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" si="9"/>
-        <v>-1884193</v>
+        <f t="shared" si="13"/>
+        <v>-804193</v>
       </c>
       <c r="K53" s="1">
         <f>ROUNDDOWN(K52+J53, 0)</f>
-        <v>1564956</v>
+        <v>2041366</v>
       </c>
       <c r="L53" s="10" t="s">
         <v>21</v>
@@ -3954,11 +3959,11 @@
         <v>1800000</v>
       </c>
       <c r="P53" s="1">
-        <f>N53-S53-T53-U53-V53-W53-O53</f>
+        <f t="shared" si="8"/>
         <v>-1250046</v>
       </c>
       <c r="Q53" s="1">
-        <f>ROUNDDOWN(Q52+P53, 0)</f>
+        <f t="shared" si="10"/>
         <v>2817783</v>
       </c>
       <c r="S53">
@@ -3974,13 +3979,13 @@
         <v>0</v>
       </c>
       <c r="W53" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="B54">
@@ -4002,20 +4007,20 @@
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="I54">
         <f>K53*0.2</f>
-        <v>312991.2</v>
+        <v>408273.2</v>
       </c>
       <c r="J54" s="1">
+        <f t="shared" si="13"/>
+        <v>-492466.2</v>
+      </c>
+      <c r="K54" s="1">
         <f t="shared" si="9"/>
-        <v>-397184.2</v>
-      </c>
-      <c r="K54" s="1">
-        <f t="shared" si="6"/>
-        <v>1167771</v>
+        <v>1548899</v>
       </c>
       <c r="L54" s="10" t="s">
         <v>14</v>
@@ -4028,11 +4033,11 @@
         <v>563556.6</v>
       </c>
       <c r="P54" s="1">
-        <f>N54-S54-T54-U54-V54-W54-O54</f>
+        <f t="shared" si="8"/>
         <v>2250.4000000000233</v>
       </c>
       <c r="Q54" s="1">
-        <f>ROUNDDOWN(Q53+P54, 0)</f>
+        <f t="shared" si="10"/>
         <v>2820033</v>
       </c>
       <c r="S54">
@@ -4048,13 +4053,13 @@
         <v>0</v>
       </c>
       <c r="W54" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="B55">
@@ -4076,7 +4081,7 @@
         <v>0</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="I55">
@@ -4084,12 +4089,12 @@
         <v>32500</v>
       </c>
       <c r="J55" s="1">
+        <f t="shared" si="13"/>
+        <v>-116693</v>
+      </c>
+      <c r="K55" s="1">
         <f t="shared" si="9"/>
-        <v>-116693</v>
-      </c>
-      <c r="K55" s="1">
-        <f t="shared" si="6"/>
-        <v>1051078</v>
+        <v>1432206</v>
       </c>
       <c r="L55" s="10" t="s">
         <v>23</v>
@@ -4102,11 +4107,11 @@
         <v>32500</v>
       </c>
       <c r="P55" s="1">
-        <f>N55-S55-T55-U55-V55-W55-O55</f>
+        <f t="shared" si="8"/>
         <v>549557</v>
       </c>
       <c r="Q55" s="1">
-        <f>ROUNDDOWN(Q54+P55, 0)</f>
+        <f t="shared" si="10"/>
         <v>3369590</v>
       </c>
       <c r="S55">
@@ -4122,13 +4127,13 @@
         <v>0</v>
       </c>
       <c r="W55" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="B56">
@@ -4150,7 +4155,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="I56">
@@ -4158,15 +4163,18 @@
         <v>1832500</v>
       </c>
       <c r="J56" s="1">
+        <f t="shared" si="13"/>
+        <v>-1916693</v>
+      </c>
+      <c r="K56" s="1">
         <f t="shared" si="9"/>
-        <v>-1916693</v>
-      </c>
-      <c r="K56" s="1">
-        <f t="shared" si="6"/>
-        <v>-865615</v>
+        <v>-484487</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>15</v>
+      </c>
+      <c r="M56" t="s">
+        <v>25</v>
       </c>
       <c r="N56" s="15">
         <v>682906</v>
@@ -4176,11 +4184,11 @@
         <v>1832500</v>
       </c>
       <c r="P56" s="1">
-        <f>N56-S56-T56-U56-V56-W56-O56</f>
+        <f t="shared" si="8"/>
         <v>-1233787</v>
       </c>
       <c r="Q56" s="1">
-        <f>ROUNDDOWN(Q55+P56, 0)</f>
+        <f t="shared" si="10"/>
         <v>2135803</v>
       </c>
       <c r="S56">
@@ -4196,13 +4204,13 @@
         <v>0</v>
       </c>
       <c r="W56" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="B57">
@@ -4224,16 +4232,16 @@
         <v>0</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J57" s="1">
+        <f t="shared" si="13"/>
+        <v>-84193</v>
+      </c>
+      <c r="K57" s="1">
         <f t="shared" si="9"/>
-        <v>-84193</v>
-      </c>
-      <c r="K57" s="1">
-        <f t="shared" si="6"/>
-        <v>-949808</v>
+        <v>-568680</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>21</v>
@@ -4242,11 +4250,11 @@
         <v>699979</v>
       </c>
       <c r="P57" s="1">
-        <f>N57-S57-T57-U57-V57-W57-O57</f>
+        <f t="shared" si="8"/>
         <v>615786</v>
       </c>
       <c r="Q57" s="1">
-        <f>ROUNDDOWN(Q56+P57, 0)</f>
+        <f t="shared" si="10"/>
         <v>2751589</v>
       </c>
       <c r="S57">
@@ -4262,13 +4270,13 @@
         <v>0</v>
       </c>
       <c r="W57" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="B58">
@@ -4290,22 +4298,22 @@
         <v>0</v>
       </c>
       <c r="H58" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J58" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-84193</v>
       </c>
       <c r="K58" s="11">
-        <f t="shared" si="2"/>
-        <v>-1034001</v>
+        <f t="shared" si="4"/>
+        <v>-652873</v>
       </c>
       <c r="N58" s="15">
         <v>717479</v>
       </c>
       <c r="P58" s="1">
-        <f>N58-S58-T58-U58-V58-W58-O58</f>
+        <f t="shared" si="8"/>
         <v>633286</v>
       </c>
       <c r="Q58" s="11">
@@ -4325,13 +4333,13 @@
         <v>0</v>
       </c>
       <c r="W58" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="B59">
@@ -4353,22 +4361,22 @@
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-84193</v>
       </c>
       <c r="K59" s="11">
-        <f t="shared" si="2"/>
-        <v>-1118194</v>
+        <f t="shared" si="4"/>
+        <v>-737066</v>
       </c>
       <c r="N59" s="15">
         <v>735416</v>
       </c>
       <c r="P59" s="1">
-        <f>N59-S59-T59-U59-V59-W59-O59</f>
+        <f t="shared" si="8"/>
         <v>651223</v>
       </c>
       <c r="Q59" s="11">
@@ -4388,13 +4396,13 @@
         <v>0</v>
       </c>
       <c r="W59" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="B60">
@@ -4416,16 +4424,16 @@
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-84193</v>
       </c>
       <c r="K60" s="11">
-        <f t="shared" si="2"/>
-        <v>-1202387</v>
+        <f t="shared" si="4"/>
+        <v>-821259</v>
       </c>
       <c r="N60" s="15">
         <v>753801</v>
@@ -4451,13 +4459,13 @@
         <v>0</v>
       </c>
       <c r="W60" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="B61">
@@ -4479,16 +4487,16 @@
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75227</v>
       </c>
       <c r="J61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-84193</v>
       </c>
       <c r="K61" s="11">
-        <f t="shared" si="2"/>
-        <v>-1286580</v>
+        <f t="shared" si="4"/>
+        <v>-905452</v>
       </c>
       <c r="N61" s="15">
         <v>772646</v>
@@ -4514,7 +4522,7 @@
         <v>0</v>
       </c>
       <c r="W61" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>75227</v>
       </c>
     </row>
@@ -4532,9 +4540,9 @@
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4545,7 +4553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4556,7 +4564,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -4568,7 +4576,7 @@
         <v>184500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A61" si="0">A3+1</f>
         <v>2</v>
@@ -4580,7 +4588,7 @@
         <v>189113</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4592,7 +4600,7 @@
         <v>193840</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4604,7 +4612,7 @@
         <v>198686</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4616,7 +4624,7 @@
         <v>203653</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4628,7 +4636,7 @@
         <v>208745</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4640,7 +4648,7 @@
         <v>213963</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4652,7 +4660,7 @@
         <v>219313</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4664,7 +4672,7 @@
         <v>224795</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4676,7 +4684,7 @@
         <v>230415</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4688,7 +4696,7 @@
         <v>236176</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4700,7 +4708,7 @@
         <v>242080</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4712,7 +4720,7 @@
         <v>248132</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4724,7 +4732,7 @@
         <v>254335</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4736,7 +4744,7 @@
         <v>260694</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4748,7 +4756,7 @@
         <v>267211</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4760,7 +4768,7 @@
         <v>273891</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4772,7 +4780,7 @@
         <v>280739</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4784,7 +4792,7 @@
         <v>287757</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4796,7 +4804,7 @@
         <v>294951</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4808,7 +4816,7 @@
         <v>302325</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4820,7 +4828,7 @@
         <v>309883</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4832,7 +4840,7 @@
         <v>317630</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4844,7 +4852,7 @@
         <v>325571</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4856,7 +4864,7 @@
         <v>333710</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4868,7 +4876,7 @@
         <v>342053</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4880,7 +4888,7 @@
         <v>350604</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4892,7 +4900,7 @@
         <v>359369</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4904,7 +4912,7 @@
         <v>368353</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4916,7 +4924,7 @@
         <v>377562</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4928,7 +4936,7 @@
         <v>387001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4940,7 +4948,7 @@
         <v>396676</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -4952,7 +4960,7 @@
         <v>406593</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -4964,7 +4972,7 @@
         <v>416758</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -4976,7 +4984,7 @@
         <v>427177</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -4988,7 +4996,7 @@
         <v>437856</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -5000,7 +5008,7 @@
         <v>448803</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -5012,7 +5020,7 @@
         <v>460023</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -5024,7 +5032,7 @@
         <v>471523</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -5036,7 +5044,7 @@
         <v>483311</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -5048,7 +5056,7 @@
         <v>495394</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -5060,7 +5068,7 @@
         <v>507779</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -5072,7 +5080,7 @@
         <v>520474</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -5084,7 +5092,7 @@
         <v>533485</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -5096,7 +5104,7 @@
         <v>546823</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -5108,7 +5116,7 @@
         <v>560493</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -5120,7 +5128,7 @@
         <v>574505</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -5132,7 +5140,7 @@
         <v>588868</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -5144,7 +5152,7 @@
         <v>603590</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -5156,7 +5164,7 @@
         <v>618680</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -5168,7 +5176,7 @@
         <v>634147</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -5180,7 +5188,7 @@
         <v>650000</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -5192,7 +5200,7 @@
         <v>666250</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -5204,7 +5212,7 @@
         <v>682906</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -5216,7 +5224,7 @@
         <v>699979</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -5228,7 +5236,7 @@
         <v>717479</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -5240,7 +5248,7 @@
         <v>735416</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -5252,7 +5260,7 @@
         <v>753801</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>

</xml_diff>

<commit_message>
updated case 1 and 2
corrected travel expense
</commit_message>
<xml_diff>
--- a/fc/Case1&2.xlsx
+++ b/fc/Case1&2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woongjin/Desktop/Projects/InsuranceGame/fc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\GoI\InsuranceGame\fc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DD8145-91E7-C24D-8079-031C5BC1DEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBB6A68-9E60-49CE-92AC-AF903D9537E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23880" yWindow="4120" windowWidth="23880" windowHeight="16180" xr2:uid="{93EEACCD-8AF9-48DF-BEAB-81301AC67219}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{93EEACCD-8AF9-48DF-BEAB-81301AC67219}"/>
   </bookViews>
   <sheets>
     <sheet name="Case_1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>step</t>
   </si>
@@ -110,9 +108,6 @@
   </si>
   <si>
     <t>Not Retired</t>
-  </si>
-  <si>
-    <t>&lt;--end</t>
   </si>
 </sst>
 </file>
@@ -623,25 +618,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AEF988-3009-472E-9717-6E6A120C3C2F}">
   <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -700,7 +695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -740,7 +735,7 @@
       <c r="V2" s="16"/>
       <c r="W2" s="16"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>1</v>
@@ -786,7 +781,7 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A61" si="3">A3+1</f>
         <v>2</v>
@@ -837,7 +832,7 @@
       <c r="V4" s="16"/>
       <c r="W4" s="16"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -888,7 +883,7 @@
       <c r="V5" s="16"/>
       <c r="W5" s="16"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -944,7 +939,7 @@
       <c r="V6" s="16"/>
       <c r="W6" s="16"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -1005,7 +1000,7 @@
       </c>
       <c r="W7" s="16"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -1066,7 +1061,7 @@
       </c>
       <c r="W8" s="16"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1127,7 +1122,7 @@
       </c>
       <c r="W9" s="16"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -1188,7 +1183,7 @@
       </c>
       <c r="W10" s="16"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1249,7 +1244,7 @@
       </c>
       <c r="W11" s="16"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1310,7 +1305,7 @@
       </c>
       <c r="W12" s="16"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1371,7 +1366,7 @@
       </c>
       <c r="W13" s="16"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -1432,7 +1427,7 @@
       </c>
       <c r="W14" s="16"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -1493,7 +1488,7 @@
       </c>
       <c r="W15" s="16"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -1554,7 +1549,7 @@
       </c>
       <c r="W16" s="16"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -1615,7 +1610,7 @@
       </c>
       <c r="W17" s="16"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -1676,7 +1671,7 @@
       </c>
       <c r="W18" s="16"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -1737,7 +1732,7 @@
       </c>
       <c r="W19" s="16"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -1803,7 +1798,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -1869,7 +1864,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -1935,7 +1930,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -2001,7 +1996,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -2067,7 +2062,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -2133,7 +2128,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -2199,7 +2194,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -2265,7 +2260,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -2331,7 +2326,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -2397,7 +2392,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -2463,7 +2458,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -2529,7 +2524,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -2595,7 +2590,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -2661,7 +2656,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -2727,7 +2722,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -2793,7 +2788,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -2859,7 +2854,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -2924,7 +2919,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -2994,7 +2989,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -3064,7 +3059,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="3"/>
         <v>38</v>
@@ -3129,7 +3124,7 @@
         <v>28074</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="3"/>
         <v>39</v>
@@ -3196,7 +3191,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="3"/>
         <v>40</v>
@@ -3270,7 +3265,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="3"/>
         <v>41</v>
@@ -3342,7 +3337,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="3"/>
         <v>42</v>
@@ -3416,7 +3411,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="3"/>
         <v>43</v>
@@ -3488,7 +3483,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="12">
         <f t="shared" si="3"/>
         <v>44</v>
@@ -3556,7 +3551,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -3623,7 +3618,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="3"/>
         <v>46</v>
@@ -3690,7 +3685,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -3762,7 +3757,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -3834,7 +3829,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -3903,7 +3898,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -3969,7 +3964,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="3"/>
         <v>51</v>
@@ -4041,7 +4036,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="3"/>
         <v>52</v>
@@ -4115,7 +4110,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="3"/>
         <v>53</v>
@@ -4187,7 +4182,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="3"/>
         <v>54</v>
@@ -4215,37 +4210,34 @@
         <v>75227</v>
       </c>
       <c r="I56">
-        <f>1800000+I55</f>
-        <v>1813325</v>
+        <f>300000+I55</f>
+        <v>313325</v>
       </c>
       <c r="J56" s="1">
         <f t="shared" si="13"/>
-        <v>-1897518</v>
+        <v>-397518</v>
       </c>
       <c r="K56" s="1">
         <f t="shared" si="9"/>
-        <v>-446136</v>
+        <v>1053864</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="M56" t="s">
-        <v>25</v>
-      </c>
       <c r="N56" s="15">
         <v>682906</v>
       </c>
       <c r="O56">
-        <f>1800000+O55</f>
-        <v>1813325</v>
+        <f>300000+O55</f>
+        <v>313325</v>
       </c>
       <c r="P56" s="1">
         <f>N56-S56-T56-U56-V56-W56-O56</f>
-        <v>-1214612</v>
+        <v>285388</v>
       </c>
       <c r="Q56" s="1">
         <f t="shared" si="10"/>
-        <v>3038153</v>
+        <v>4538153</v>
       </c>
       <c r="S56">
         <v>5040</v>
@@ -4264,7 +4256,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="3"/>
         <v>55</v>
@@ -4297,7 +4289,7 @@
       </c>
       <c r="K57" s="1">
         <f t="shared" si="9"/>
-        <v>-530329</v>
+        <v>969671</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>19</v>
@@ -4315,7 +4307,7 @@
       </c>
       <c r="Q57" s="1">
         <f t="shared" si="10"/>
-        <v>3640614</v>
+        <v>5140614</v>
       </c>
       <c r="S57">
         <v>5040</v>
@@ -4334,7 +4326,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="3"/>
         <v>56</v>
@@ -4367,7 +4359,7 @@
       </c>
       <c r="K58" s="11">
         <f t="shared" si="4"/>
-        <v>-614522</v>
+        <v>885478</v>
       </c>
       <c r="L58" t="s">
         <v>21</v>
@@ -4385,7 +4377,7 @@
       </c>
       <c r="Q58" s="11">
         <f>Q57+P58</f>
-        <v>3540575</v>
+        <v>5040575</v>
       </c>
       <c r="S58">
         <v>5040</v>
@@ -4404,7 +4396,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="3"/>
         <v>57</v>
@@ -4437,7 +4429,7 @@
       </c>
       <c r="K59" s="11">
         <f t="shared" si="4"/>
-        <v>-698715</v>
+        <v>801285</v>
       </c>
       <c r="L59" t="s">
         <v>15</v>
@@ -4446,16 +4438,16 @@
         <v>735416</v>
       </c>
       <c r="O59">
-        <f>1800000+O55</f>
-        <v>1813325</v>
+        <f>300000+O55</f>
+        <v>313325</v>
       </c>
       <c r="P59" s="1">
         <f t="shared" si="8"/>
-        <v>-1162102</v>
+        <v>337898</v>
       </c>
       <c r="Q59" s="11">
         <f>Q58+P59</f>
-        <v>2378473</v>
+        <v>5378473</v>
       </c>
       <c r="S59">
         <v>5040</v>
@@ -4474,7 +4466,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="3"/>
         <v>58</v>
@@ -4507,7 +4499,7 @@
       </c>
       <c r="K60" s="11">
         <f t="shared" si="4"/>
-        <v>-782908</v>
+        <v>717092</v>
       </c>
       <c r="L60" t="s">
         <v>20</v>
@@ -4525,7 +4517,7 @@
       </c>
       <c r="Q60" s="11">
         <f>Q59+P60</f>
-        <v>3048081</v>
+        <v>6048081</v>
       </c>
       <c r="S60">
         <v>5040</v>
@@ -4544,7 +4536,7 @@
         <v>75227</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="3"/>
         <v>59</v>
@@ -4577,7 +4569,7 @@
       </c>
       <c r="K61" s="11">
         <f t="shared" si="4"/>
-        <v>-867101</v>
+        <v>632899</v>
       </c>
       <c r="L61" t="s">
         <v>10</v>
@@ -4595,7 +4587,7 @@
       </c>
       <c r="Q61" s="11">
         <f>Q60+P61</f>
-        <v>3736534</v>
+        <v>6736534</v>
       </c>
       <c r="S61">
         <v>5040</v>
@@ -4628,9 +4620,9 @@
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4641,7 +4633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4652,7 +4644,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -4664,7 +4656,7 @@
         <v>184500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A61" si="0">A3+1</f>
         <v>2</v>
@@ -4676,7 +4668,7 @@
         <v>189113</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4688,7 +4680,7 @@
         <v>193840</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4700,7 +4692,7 @@
         <v>198686</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4712,7 +4704,7 @@
         <v>203653</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4724,7 +4716,7 @@
         <v>208745</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4736,7 +4728,7 @@
         <v>213963</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4748,7 +4740,7 @@
         <v>219313</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4760,7 +4752,7 @@
         <v>224795</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4772,7 +4764,7 @@
         <v>230415</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4784,7 +4776,7 @@
         <v>236176</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4796,7 +4788,7 @@
         <v>242080</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4808,7 +4800,7 @@
         <v>248132</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4820,7 +4812,7 @@
         <v>254335</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4832,7 +4824,7 @@
         <v>260694</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4844,7 +4836,7 @@
         <v>267211</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4856,7 +4848,7 @@
         <v>273891</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4868,7 +4860,7 @@
         <v>280739</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4880,7 +4872,7 @@
         <v>287757</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4892,7 +4884,7 @@
         <v>294951</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4904,7 +4896,7 @@
         <v>302325</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4916,7 +4908,7 @@
         <v>309883</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4928,7 +4920,7 @@
         <v>317630</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4940,7 +4932,7 @@
         <v>325571</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4952,7 +4944,7 @@
         <v>333710</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4964,7 +4956,7 @@
         <v>342053</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4976,7 +4968,7 @@
         <v>350604</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4988,7 +4980,7 @@
         <v>359369</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -5000,7 +4992,7 @@
         <v>368353</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5012,7 +5004,7 @@
         <v>377562</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -5024,7 +5016,7 @@
         <v>387001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -5036,7 +5028,7 @@
         <v>396676</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -5048,7 +5040,7 @@
         <v>406593</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -5060,7 +5052,7 @@
         <v>416758</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -5072,7 +5064,7 @@
         <v>427177</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -5084,7 +5076,7 @@
         <v>437856</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -5096,7 +5088,7 @@
         <v>448803</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -5108,7 +5100,7 @@
         <v>460023</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -5120,7 +5112,7 @@
         <v>471523</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -5132,7 +5124,7 @@
         <v>483311</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -5144,7 +5136,7 @@
         <v>495394</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -5156,7 +5148,7 @@
         <v>507779</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -5168,7 +5160,7 @@
         <v>520474</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -5180,7 +5172,7 @@
         <v>533485</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -5192,7 +5184,7 @@
         <v>546823</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -5204,7 +5196,7 @@
         <v>560493</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -5216,7 +5208,7 @@
         <v>574505</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -5228,7 +5220,7 @@
         <v>588868</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -5240,7 +5232,7 @@
         <v>603590</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -5252,7 +5244,7 @@
         <v>618680</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -5264,7 +5256,7 @@
         <v>634147</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -5276,7 +5268,7 @@
         <v>650000</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -5288,7 +5280,7 @@
         <v>666250</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -5300,7 +5292,7 @@
         <v>682906</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -5312,7 +5304,7 @@
         <v>699979</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -5324,7 +5316,7 @@
         <v>717479</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -5336,7 +5328,7 @@
         <v>735416</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -5348,7 +5340,7 @@
         <v>753801</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>

</xml_diff>